<commit_message>
Quitado entorno EXCEL y Activado MENU APP y Atajos Teclados
</commit_message>
<xml_diff>
--- a/FastTest PlugIn - Formula.xlsx
+++ b/FastTest PlugIn - Formula.xlsx
@@ -80,6 +80,9 @@
     <definedName name="Dato_06" localSheetId="6">'Formulas PP'!$Y$15</definedName>
     <definedName name="Dato_06" localSheetId="5">'Formulas RC'!$Y$15</definedName>
     <definedName name="Dato_06" localSheetId="3">'Formulas VF'!$Y$15</definedName>
+    <definedName name="Dato_07" localSheetId="8">'Formulas CL'!$Y$17</definedName>
+    <definedName name="Dato_07" localSheetId="1">'Formulas OM'!$Y$17</definedName>
+    <definedName name="Dato_08" localSheetId="8">'Formulas CL'!$Y$19</definedName>
     <definedName name="Dato_10" localSheetId="8">'Formulas CL'!$Y$23</definedName>
     <definedName name="Dato_10" localSheetId="0">'Formulas DG'!$Y$23</definedName>
     <definedName name="Dato_10" localSheetId="4">'Formulas EM'!$Y$23</definedName>
@@ -188,9 +191,10 @@
     <definedName name="Dato_25" localSheetId="6">'Formulas PP'!$AA$21</definedName>
     <definedName name="Dato_25" localSheetId="5">'Formulas RC'!$AA$21</definedName>
     <definedName name="Dato_25" localSheetId="3">'Formulas VF'!$AA$21</definedName>
+    <definedName name="Dato_32" localSheetId="8">'Formulas CL'!$AA$35</definedName>
     <definedName name="IDIOMA">[1]INICIO!$A$37</definedName>
-    <definedName name="P_max_CL">'[1]DATOS GENERALES'!$N$45</definedName>
-    <definedName name="P_min_CL">'[1]DATOS GENERALES'!$M$45</definedName>
+    <definedName name="P_max_CL">#REF!</definedName>
+    <definedName name="P_min_CL">#REF!</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -202,7 +206,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="167">
   <si>
     <t>DATO_01</t>
   </si>
@@ -570,9 +574,6 @@
     <t>VARIABLES</t>
   </si>
   <si>
-    <t>V5.0</t>
-  </si>
-  <si>
     <t>DATOS GENERALES</t>
   </si>
   <si>
@@ -666,43 +667,46 @@
     <t>Categ_20</t>
   </si>
   <si>
-    <t>SubCat_22</t>
-  </si>
-  <si>
-    <t>SubCat_21</t>
-  </si>
-  <si>
-    <t>SubCat_23</t>
-  </si>
-  <si>
-    <t>SubCat_24</t>
-  </si>
-  <si>
-    <t>SubCat_25</t>
-  </si>
-  <si>
-    <t>SubCat_26</t>
-  </si>
-  <si>
-    <t>SubCat_27</t>
-  </si>
-  <si>
-    <t>SubCat_28</t>
-  </si>
-  <si>
-    <t>SubCat_29</t>
-  </si>
-  <si>
-    <t>SubCat_30</t>
-  </si>
-  <si>
-    <t>SubCat_31</t>
-  </si>
-  <si>
-    <t>SubCat_32</t>
-  </si>
-  <si>
     <t>Mensaje Marcar Texto</t>
+  </si>
+  <si>
+    <t>SubCat_01</t>
+  </si>
+  <si>
+    <t>SubCat_02</t>
+  </si>
+  <si>
+    <t>SubCat_03</t>
+  </si>
+  <si>
+    <t>SubCat_04</t>
+  </si>
+  <si>
+    <t>SubCat_05</t>
+  </si>
+  <si>
+    <t>SubCat_06</t>
+  </si>
+  <si>
+    <t>SubCat_07</t>
+  </si>
+  <si>
+    <t>SubCat_08</t>
+  </si>
+  <si>
+    <t>SubCat_09</t>
+  </si>
+  <si>
+    <t>SubCat_10</t>
+  </si>
+  <si>
+    <t>SubCat_11</t>
+  </si>
+  <si>
+    <t>SubCat_12</t>
+  </si>
+  <si>
+    <t>V6.0</t>
   </si>
 </sst>
 </file>
@@ -1028,7 +1032,7 @@
     <sheetNames>
       <sheetName val="DICCIONARIO"/>
       <sheetName val="INICIO"/>
-      <sheetName val="DATOS GENERALES"/>
+      <sheetName val="GENERAL"/>
       <sheetName val="Formulario OM"/>
       <sheetName val="Datos OM"/>
       <sheetName val="Formulario O2"/>
@@ -1058,6 +1062,7 @@
       <sheetName val="DOC_2"/>
       <sheetName val="DOC_TEMP"/>
       <sheetName val="OCA"/>
+      <sheetName val="DATOS GENERALES"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0"/>
@@ -1068,16 +1073,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2">
-        <row r="45">
-          <cell r="M45">
-            <v>0</v>
-          </cell>
-          <cell r="N45">
-            <v>0</v>
-          </cell>
-        </row>
-      </sheetData>
+      <sheetData sheetId="2"/>
       <sheetData sheetId="3"/>
       <sheetData sheetId="4"/>
       <sheetData sheetId="5"/>
@@ -1107,6 +1103,13 @@
       <sheetData sheetId="29"/>
       <sheetData sheetId="30"/>
       <sheetData sheetId="31"/>
+      <sheetData sheetId="32">
+        <row r="45">
+          <cell r="M45">
+            <v>0</v>
+          </cell>
+        </row>
+      </sheetData>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1434,10 +1437,10 @@
     </row>
     <row r="5" spans="1:34" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="26" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="AC5" s="7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="AD5" s="8"/>
       <c r="AE5" s="8"/>
@@ -1448,7 +1451,7 @@
     <row r="6" spans="1:34" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="26"/>
       <c r="AC6" s="9" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="AD6" s="10"/>
       <c r="AE6" s="10"/>
@@ -1459,7 +1462,7 @@
     <row r="7" spans="1:34" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="26"/>
       <c r="AC7" s="9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="AD7" s="10"/>
       <c r="AE7" s="10"/>
@@ -1470,7 +1473,7 @@
     <row r="8" spans="1:34" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="26"/>
       <c r="AC8" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="AD8" s="10"/>
       <c r="AE8" s="10"/>
@@ -1481,7 +1484,7 @@
     <row r="9" spans="1:34" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="26"/>
       <c r="AC9" s="9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="AD9" s="10"/>
       <c r="AE9" s="10"/>
@@ -1492,7 +1495,7 @@
     <row r="10" spans="1:34" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="26"/>
       <c r="AC10" s="9" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AD10" s="10"/>
       <c r="AE10" s="10"/>
@@ -1503,7 +1506,7 @@
     <row r="11" spans="1:34" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="26"/>
       <c r="AC11" s="9" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AD11" s="10"/>
       <c r="AE11" s="10"/>
@@ -1514,7 +1517,7 @@
     <row r="12" spans="1:34" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="26"/>
       <c r="AC12" s="9" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AD12" s="10"/>
       <c r="AE12" s="10"/>
@@ -1525,7 +1528,7 @@
     <row r="13" spans="1:34" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="26"/>
       <c r="AC13" s="9" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="AD13" s="10"/>
       <c r="AE13" s="10"/>
@@ -1536,7 +1539,7 @@
     <row r="14" spans="1:34" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="26"/>
       <c r="AC14" s="9" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AD14" s="10"/>
       <c r="AE14" s="10"/>
@@ -1547,7 +1550,7 @@
     <row r="15" spans="1:34" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="26"/>
       <c r="AC15" s="9" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="AD15" s="10"/>
       <c r="AE15" s="10"/>
@@ -1558,7 +1561,7 @@
     <row r="16" spans="1:34" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="26"/>
       <c r="AC16" s="9" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AD16" s="10"/>
       <c r="AE16" s="10"/>
@@ -1569,7 +1572,7 @@
     <row r="17" spans="1:34" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="26"/>
       <c r="AC17" s="9" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="AD17" s="10"/>
       <c r="AE17" s="10"/>
@@ -1580,7 +1583,7 @@
     <row r="18" spans="1:34" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="26"/>
       <c r="AC18" s="9" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="AD18" s="10"/>
       <c r="AE18" s="10"/>
@@ -1591,7 +1594,7 @@
     <row r="19" spans="1:34" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="26"/>
       <c r="AC19" s="9" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="AD19" s="10"/>
       <c r="AE19" s="10"/>
@@ -1602,7 +1605,7 @@
     <row r="20" spans="1:34" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="26"/>
       <c r="AC20" s="9" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="AD20" s="10"/>
       <c r="AE20" s="10"/>
@@ -1612,10 +1615,10 @@
     </row>
     <row r="21" spans="1:34" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="26" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="AC21" s="9" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="AD21" s="10"/>
       <c r="AE21" s="10"/>
@@ -1626,7 +1629,7 @@
     <row r="22" spans="1:34" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="26"/>
       <c r="AC22" s="9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="AD22" s="10"/>
       <c r="AE22" s="10"/>
@@ -1637,7 +1640,7 @@
     <row r="23" spans="1:34" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="26"/>
       <c r="AC23" s="9" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="AD23" s="10"/>
       <c r="AE23" s="10"/>
@@ -1647,30 +1650,30 @@
     </row>
     <row r="24" spans="1:34" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="26"/>
-      <c r="AC24" s="9" t="s">
-        <v>153</v>
-      </c>
-      <c r="AD24" s="10"/>
-      <c r="AE24" s="10"/>
-      <c r="AF24" s="10"/>
-      <c r="AG24" s="10"/>
-      <c r="AH24" s="10"/>
+      <c r="AC24" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="AD24" s="12"/>
+      <c r="AE24" s="12"/>
+      <c r="AF24" s="12"/>
+      <c r="AG24" s="12"/>
+      <c r="AH24" s="12"/>
     </row>
     <row r="25" spans="1:34" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="26"/>
-      <c r="AC25" s="9" t="s">
-        <v>155</v>
-      </c>
-      <c r="AD25" s="10"/>
-      <c r="AE25" s="10"/>
-      <c r="AF25" s="10"/>
-      <c r="AG25" s="10"/>
-      <c r="AH25" s="10"/>
+      <c r="AC25" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="AD25" s="8"/>
+      <c r="AE25" s="8"/>
+      <c r="AF25" s="8"/>
+      <c r="AG25" s="8"/>
+      <c r="AH25" s="8"/>
     </row>
     <row r="26" spans="1:34" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="26"/>
       <c r="AC26" s="9" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="AD26" s="10"/>
       <c r="AE26" s="10"/>
@@ -1790,7 +1793,7 @@
     </row>
     <row r="37" spans="1:34" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="25" t="s">
-        <v>122</v>
+        <v>166</v>
       </c>
       <c r="AC37" s="2"/>
       <c r="AD37" s="17"/>
@@ -1811,7 +1814,7 @@
     </row>
     <row r="39" spans="1:34" x14ac:dyDescent="0.25">
       <c r="AC39" s="13" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="AD39" s="8"/>
       <c r="AE39" s="8"/>
@@ -1821,7 +1824,7 @@
     </row>
     <row r="40" spans="1:34" x14ac:dyDescent="0.25">
       <c r="AC40" s="14" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="AD40" s="10"/>
       <c r="AE40" s="10"/>
@@ -1831,7 +1834,7 @@
     </row>
     <row r="41" spans="1:34" x14ac:dyDescent="0.25">
       <c r="AC41" s="14" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="AD41" s="10"/>
       <c r="AE41" s="10"/>
@@ -1841,7 +1844,7 @@
     </row>
     <row r="42" spans="1:34" x14ac:dyDescent="0.25">
       <c r="AC42" s="14" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="AD42" s="10"/>
       <c r="AE42" s="10"/>
@@ -1851,7 +1854,7 @@
     </row>
     <row r="43" spans="1:34" x14ac:dyDescent="0.25">
       <c r="AC43" s="14" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="AD43" s="10"/>
       <c r="AE43" s="10"/>
@@ -1861,7 +1864,7 @@
     </row>
     <row r="44" spans="1:34" x14ac:dyDescent="0.25">
       <c r="AC44" s="14" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="AD44" s="10"/>
       <c r="AE44" s="10"/>
@@ -1871,7 +1874,7 @@
     </row>
     <row r="45" spans="1:34" x14ac:dyDescent="0.25">
       <c r="AC45" s="14" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AD45" s="10"/>
       <c r="AE45" s="10"/>
@@ -1881,7 +1884,7 @@
     </row>
     <row r="46" spans="1:34" x14ac:dyDescent="0.25">
       <c r="AC46" s="14" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="AD46" s="10"/>
       <c r="AE46" s="10"/>
@@ -1891,7 +1894,7 @@
     </row>
     <row r="47" spans="1:34" x14ac:dyDescent="0.25">
       <c r="AC47" s="14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="AD47" s="10"/>
       <c r="AE47" s="10"/>
@@ -1901,7 +1904,7 @@
     </row>
     <row r="48" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="AC48" s="15" t="s">
-        <v>166</v>
+        <v>153</v>
       </c>
       <c r="AD48" s="12"/>
       <c r="AE48" s="12"/>
@@ -1973,23 +1976,23 @@
     <row r="110" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="111" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="112" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="113" x14ac:dyDescent="0.25"/>
-    <row r="114" x14ac:dyDescent="0.25"/>
-    <row r="115" x14ac:dyDescent="0.25"/>
-    <row r="116" x14ac:dyDescent="0.25"/>
-    <row r="117" x14ac:dyDescent="0.25"/>
-    <row r="118" x14ac:dyDescent="0.25"/>
-    <row r="119" x14ac:dyDescent="0.25"/>
-    <row r="120" x14ac:dyDescent="0.25"/>
-    <row r="121" x14ac:dyDescent="0.25"/>
-    <row r="122" x14ac:dyDescent="0.25"/>
-    <row r="123" x14ac:dyDescent="0.25"/>
-    <row r="124" x14ac:dyDescent="0.25"/>
-    <row r="125" x14ac:dyDescent="0.25"/>
-    <row r="126" x14ac:dyDescent="0.25"/>
-    <row r="127" x14ac:dyDescent="0.25"/>
+    <row r="113" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="114" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="115" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="116" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="117" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="118" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="119" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="120" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="121" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="122" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="123" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="124" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="125" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="126" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="127" hidden="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="lQJM93IZQVvsa3mQ0pAL5Xrp/18hFYOUqwCrXUHc5y3TEcnRPITQRsJxBgtubSQ6UxPVbE4Hxu19a5USj1f8ng==" saltValue="iXxrlJRzf3Us6hcEg3HvxQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="z3gvLj4K+7/e8fdl3C2xyAeWZFp17aI8GfDWfvB/XB+CP8QYpXay9CCwc1PkjnsNMGeugFtbUJ4sQelsfTHy6A==" saltValue="VH3amv1o2NFKWyeGOTuuag==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="2">
     <mergeCell ref="A5:A20"/>
     <mergeCell ref="A21:A36"/>
@@ -2415,8 +2418,9 @@
       <c r="AH36" s="12"/>
     </row>
     <row r="37" spans="1:34" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="25" t="s">
-        <v>122</v>
+      <c r="A37" s="25" t="str">
+        <f>'Formulas DG'!A37</f>
+        <v>V6.0</v>
       </c>
       <c r="AC37" s="2"/>
       <c r="AD37" s="17"/>
@@ -2750,7 +2754,7 @@
     <row r="126" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="127" hidden="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="FjW+cIVNWnPoD74dezG2D2NTdegvC2wkmIFXt9FGlkt5os03KKQmydaMqsnKksCoNAKg8pa+zJ4utmD+Pvm8zw==" saltValue="QixaBhNemKAxXq+2MZ6viQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="ggCFnJrWvtpZWMJctKTCvtWqk9z2Hdgi17AJjSahZ6yE2WdkzHvh3TfRd3dLqiVkN2ZyeX11xffFR7wiVjtV2A==" saltValue="VQqcffabnjBdJcU3aCRYew==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="2">
     <mergeCell ref="A5:A20"/>
     <mergeCell ref="A21:A36"/>
@@ -3178,7 +3182,7 @@
     <row r="37" spans="1:34" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="25" t="str">
         <f>'Formulas OM'!A37</f>
-        <v>V5.0</v>
+        <v>V6.0</v>
       </c>
       <c r="AC37" s="2"/>
       <c r="AD37" s="17"/>
@@ -3939,7 +3943,7 @@
     <row r="37" spans="1:34" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="25" t="str">
         <f>'Formulas OM'!A37</f>
-        <v>V5.0</v>
+        <v>V6.0</v>
       </c>
       <c r="AC37" s="2"/>
       <c r="AD37" s="17"/>
@@ -4157,7 +4161,7 @@
       <selection activeCell="AC48" sqref="AC48"/>
       <selection pane="topRight" activeCell="AC48" sqref="AC48"/>
       <selection pane="bottomLeft" activeCell="AC48" sqref="AC48"/>
-      <selection pane="bottomRight" activeCell="AD5" sqref="AD5"/>
+      <selection pane="bottomRight" activeCell="AD6" sqref="AD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -4565,7 +4569,7 @@
     <row r="37" spans="1:34" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="25" t="str">
         <f>'Formulas OM'!A37</f>
-        <v>V5.0</v>
+        <v>V6.0</v>
       </c>
       <c r="AC37" s="2"/>
       <c r="AD37" s="17"/>
@@ -4975,7 +4979,7 @@
       <selection activeCell="AC48" sqref="AC48"/>
       <selection pane="topRight" activeCell="AC48" sqref="AC48"/>
       <selection pane="bottomLeft" activeCell="AC48" sqref="AC48"/>
-      <selection pane="bottomRight" activeCell="AD5" sqref="AD5"/>
+      <selection pane="bottomRight" activeCell="AD6" sqref="AD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -5383,7 +5387,7 @@
     <row r="37" spans="1:34" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="25" t="str">
         <f>'Formulas OM'!A37</f>
-        <v>V5.0</v>
+        <v>V6.0</v>
       </c>
       <c r="AC37" s="2"/>
       <c r="AD37" s="17"/>
@@ -5801,7 +5805,7 @@
       <selection activeCell="AC48" sqref="AC48"/>
       <selection pane="topRight" activeCell="AC48" sqref="AC48"/>
       <selection pane="bottomLeft" activeCell="AC48" sqref="AC48"/>
-      <selection pane="bottomRight" activeCell="AD5" sqref="AD5"/>
+      <selection pane="bottomRight" activeCell="AD6" sqref="AD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -6209,7 +6213,7 @@
     <row r="37" spans="1:34" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="25" t="str">
         <f>'Formulas OM'!A37</f>
-        <v>V5.0</v>
+        <v>V6.0</v>
       </c>
       <c r="AC37" s="2"/>
       <c r="AD37" s="17"/>
@@ -6616,7 +6620,7 @@
       <selection activeCell="AC48" sqref="AC48"/>
       <selection pane="topRight" activeCell="AC48" sqref="AC48"/>
       <selection pane="bottomLeft" activeCell="AC48" sqref="AC48"/>
-      <selection pane="bottomRight" activeCell="AD5" sqref="AD5"/>
+      <selection pane="bottomRight" activeCell="AD6" sqref="AD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -7024,7 +7028,7 @@
     <row r="37" spans="1:34" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="25" t="str">
         <f>'Formulas OM'!A37</f>
-        <v>V5.0</v>
+        <v>V6.0</v>
       </c>
       <c r="AC37" s="2"/>
       <c r="AD37" s="17"/>
@@ -7650,7 +7654,7 @@
     <row r="37" spans="1:34" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="25" t="str">
         <f>'Formulas OM'!A37</f>
-        <v>V5.0</v>
+        <v>V6.0</v>
       </c>
       <c r="AC37" s="2"/>
       <c r="AD37" s="17"/>
@@ -7703,7 +7707,7 @@
       <c r="AC42" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="AD42" s="10"/>
+      <c r="AD42" s="21"/>
       <c r="AE42" s="21"/>
       <c r="AF42" s="21"/>
       <c r="AG42" s="21"/>

</xml_diff>

<commit_message>
Arreglos varios, incluida hoja de Problemas Tipo
</commit_message>
<xml_diff>
--- a/FastTest PlugIn - Formula.xlsx
+++ b/FastTest PlugIn - Formula.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\milag\Desktop\FastTest PlugIn\z. V7.7\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Mi unidad\FTP\z. V8.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{731D7D46-11AB-4E8C-B4BA-9AC676741BCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4734179-7E05-4920-A1A9-28C7F7BBD236}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-93" yWindow="-93" windowWidth="19386" windowHeight="12266" tabRatio="805" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,184 +23,6 @@
     <sheet name="Formulas EN" sheetId="5" r:id="rId8"/>
     <sheet name="Formulas CL" sheetId="6" r:id="rId9"/>
   </sheets>
-  <definedNames>
-    <definedName name="Dato_01" localSheetId="8">'Formulas CL'!$Y$5</definedName>
-    <definedName name="Dato_01" localSheetId="0">'Formulas DG'!$Y$5</definedName>
-    <definedName name="Dato_01" localSheetId="4">'Formulas EM'!$Y$5</definedName>
-    <definedName name="Dato_01" localSheetId="7">'Formulas EN'!$Y$5</definedName>
-    <definedName name="Dato_01" localSheetId="2">'Formulas O2'!$Y$5</definedName>
-    <definedName name="Dato_01" localSheetId="1">'Formulas OM'!$Y$5</definedName>
-    <definedName name="Dato_01" localSheetId="6">'Formulas PP'!$Y$5</definedName>
-    <definedName name="Dato_01" localSheetId="5">'Formulas RC'!$Y$5</definedName>
-    <definedName name="Dato_01" localSheetId="3">'Formulas VF'!$Y$5</definedName>
-    <definedName name="Dato_02" localSheetId="8">'Formulas CL'!$Y$7</definedName>
-    <definedName name="Dato_02" localSheetId="0">'Formulas DG'!$Y$7</definedName>
-    <definedName name="Dato_02" localSheetId="4">'Formulas EM'!$Y$7</definedName>
-    <definedName name="Dato_02" localSheetId="7">'Formulas EN'!$Y$7</definedName>
-    <definedName name="Dato_02" localSheetId="2">'Formulas O2'!$Y$7</definedName>
-    <definedName name="Dato_02" localSheetId="1">'Formulas OM'!$Y$7</definedName>
-    <definedName name="Dato_02" localSheetId="6">'Formulas PP'!$Y$7</definedName>
-    <definedName name="Dato_02" localSheetId="5">'Formulas RC'!$Y$7</definedName>
-    <definedName name="Dato_02" localSheetId="3">'Formulas VF'!$Y$7</definedName>
-    <definedName name="Dato_03" localSheetId="8">'Formulas CL'!$Y$9</definedName>
-    <definedName name="Dato_03" localSheetId="0">'Formulas DG'!$Y$9</definedName>
-    <definedName name="Dato_03" localSheetId="4">'Formulas EM'!$Y$9</definedName>
-    <definedName name="Dato_03" localSheetId="7">'Formulas EN'!$Y$9</definedName>
-    <definedName name="Dato_03" localSheetId="2">'Formulas O2'!$Y$9</definedName>
-    <definedName name="Dato_03" localSheetId="1">'Formulas OM'!$Y$9</definedName>
-    <definedName name="Dato_03" localSheetId="6">'Formulas PP'!$Y$9</definedName>
-    <definedName name="Dato_03" localSheetId="5">'Formulas RC'!$Y$9</definedName>
-    <definedName name="Dato_03" localSheetId="3">'Formulas VF'!$Y$9</definedName>
-    <definedName name="Dato_04" localSheetId="8">'Formulas CL'!$Y$11</definedName>
-    <definedName name="Dato_04" localSheetId="0">'Formulas DG'!$Y$11</definedName>
-    <definedName name="Dato_04" localSheetId="4">'Formulas EM'!$Y$11</definedName>
-    <definedName name="Dato_04" localSheetId="7">'Formulas EN'!$Y$11</definedName>
-    <definedName name="Dato_04" localSheetId="2">'Formulas O2'!$Y$11</definedName>
-    <definedName name="Dato_04" localSheetId="1">'Formulas OM'!$Y$11</definedName>
-    <definedName name="Dato_04" localSheetId="6">'Formulas PP'!$Y$11</definedName>
-    <definedName name="Dato_04" localSheetId="5">'Formulas RC'!$Y$11</definedName>
-    <definedName name="Dato_04" localSheetId="3">'Formulas VF'!$Y$11</definedName>
-    <definedName name="Dato_05" localSheetId="8">'Formulas CL'!$Y$13</definedName>
-    <definedName name="Dato_05" localSheetId="0">'Formulas DG'!$Y$13</definedName>
-    <definedName name="Dato_05" localSheetId="4">'Formulas EM'!$Y$13</definedName>
-    <definedName name="Dato_05" localSheetId="7">'Formulas EN'!$Y$13</definedName>
-    <definedName name="Dato_05" localSheetId="2">'Formulas O2'!$Y$13</definedName>
-    <definedName name="Dato_05" localSheetId="1">'Formulas OM'!$Y$13</definedName>
-    <definedName name="Dato_05" localSheetId="6">'Formulas PP'!$Y$13</definedName>
-    <definedName name="Dato_05" localSheetId="5">'Formulas RC'!$Y$13</definedName>
-    <definedName name="Dato_05" localSheetId="3">'Formulas VF'!$Y$13</definedName>
-    <definedName name="Dato_06" localSheetId="8">'Formulas CL'!$Y$15</definedName>
-    <definedName name="Dato_06" localSheetId="0">'Formulas DG'!$Y$15</definedName>
-    <definedName name="Dato_06" localSheetId="4">'Formulas EM'!$Y$15</definedName>
-    <definedName name="Dato_06" localSheetId="7">'Formulas EN'!$Y$15</definedName>
-    <definedName name="Dato_06" localSheetId="2">'Formulas O2'!$Y$15</definedName>
-    <definedName name="Dato_06" localSheetId="1">'Formulas OM'!$Y$15</definedName>
-    <definedName name="Dato_06" localSheetId="6">'Formulas PP'!$Y$15</definedName>
-    <definedName name="Dato_06" localSheetId="5">'Formulas RC'!$Y$15</definedName>
-    <definedName name="Dato_06" localSheetId="3">'Formulas VF'!$Y$15</definedName>
-    <definedName name="Dato_07" localSheetId="8">'Formulas CL'!$Y$17</definedName>
-    <definedName name="Dato_07" localSheetId="1">'Formulas OM'!$Y$17</definedName>
-    <definedName name="Dato_08" localSheetId="8">'Formulas CL'!$Y$19</definedName>
-    <definedName name="Dato_10" localSheetId="8">'Formulas CL'!$Y$23</definedName>
-    <definedName name="Dato_10" localSheetId="0">'Formulas DG'!$Y$23</definedName>
-    <definedName name="Dato_10" localSheetId="4">'Formulas EM'!$Y$23</definedName>
-    <definedName name="Dato_10" localSheetId="7">'Formulas EN'!$Y$23</definedName>
-    <definedName name="Dato_10" localSheetId="2">'Formulas O2'!$Y$23</definedName>
-    <definedName name="Dato_10" localSheetId="1">'Formulas OM'!$Y$23</definedName>
-    <definedName name="Dato_10" localSheetId="6">'Formulas PP'!$Y$23</definedName>
-    <definedName name="Dato_10" localSheetId="5">'Formulas RC'!$Y$23</definedName>
-    <definedName name="Dato_10" localSheetId="3">'Formulas VF'!$Y$23</definedName>
-    <definedName name="Dato_11" localSheetId="8">'Formulas CL'!$Y$25</definedName>
-    <definedName name="Dato_11" localSheetId="0">'Formulas DG'!$Y$25</definedName>
-    <definedName name="Dato_11" localSheetId="4">'Formulas EM'!$Y$25</definedName>
-    <definedName name="Dato_11" localSheetId="7">'Formulas EN'!$Y$25</definedName>
-    <definedName name="Dato_11" localSheetId="2">'Formulas O2'!$Y$25</definedName>
-    <definedName name="Dato_11" localSheetId="1">'Formulas OM'!$Y$25</definedName>
-    <definedName name="Dato_11" localSheetId="6">'Formulas PP'!$Y$25</definedName>
-    <definedName name="Dato_11" localSheetId="5">'Formulas RC'!$Y$25</definedName>
-    <definedName name="Dato_11" localSheetId="3">'Formulas VF'!$Y$25</definedName>
-    <definedName name="Dato_12" localSheetId="8">'Formulas CL'!$Y$27</definedName>
-    <definedName name="Dato_12" localSheetId="0">'Formulas DG'!$Y$27</definedName>
-    <definedName name="Dato_12" localSheetId="4">'Formulas EM'!$Y$27</definedName>
-    <definedName name="Dato_12" localSheetId="7">'Formulas EN'!$Y$27</definedName>
-    <definedName name="Dato_12" localSheetId="2">'Formulas O2'!$Y$27</definedName>
-    <definedName name="Dato_12" localSheetId="1">'Formulas OM'!$Y$27</definedName>
-    <definedName name="Dato_12" localSheetId="6">'Formulas PP'!$Y$27</definedName>
-    <definedName name="Dato_12" localSheetId="5">'Formulas RC'!$Y$27</definedName>
-    <definedName name="Dato_12" localSheetId="3">'Formulas VF'!$Y$27</definedName>
-    <definedName name="Dato_13" localSheetId="8">'Formulas CL'!$Y$29</definedName>
-    <definedName name="Dato_14" localSheetId="8">'Formulas CL'!$Y$31</definedName>
-    <definedName name="Dato_15" localSheetId="8">'Formulas CL'!$Y$33</definedName>
-    <definedName name="Dato_16" localSheetId="8">'Formulas CL'!$Y$35</definedName>
-    <definedName name="Dato_17" localSheetId="8">'Formulas CL'!$AA$5</definedName>
-    <definedName name="Dato_17" localSheetId="0">'Formulas DG'!$AA$5</definedName>
-    <definedName name="Dato_17" localSheetId="4">'Formulas EM'!$AA$5</definedName>
-    <definedName name="Dato_17" localSheetId="7">'Formulas EN'!$AA$5</definedName>
-    <definedName name="Dato_17" localSheetId="2">'Formulas O2'!$AA$5</definedName>
-    <definedName name="Dato_17" localSheetId="1">'Formulas OM'!$AA$5</definedName>
-    <definedName name="Dato_17" localSheetId="6">'Formulas PP'!$AA$5</definedName>
-    <definedName name="Dato_17" localSheetId="5">'Formulas RC'!$AA$5</definedName>
-    <definedName name="Dato_17" localSheetId="3">'Formulas VF'!$AA$5</definedName>
-    <definedName name="Dato_18" localSheetId="8">'Formulas CL'!$AA$7</definedName>
-    <definedName name="Dato_18" localSheetId="0">'Formulas DG'!$AA$7</definedName>
-    <definedName name="Dato_18" localSheetId="4">'Formulas EM'!$AA$7</definedName>
-    <definedName name="Dato_18" localSheetId="7">'Formulas EN'!$AA$7</definedName>
-    <definedName name="Dato_18" localSheetId="2">'Formulas O2'!$AA$7</definedName>
-    <definedName name="Dato_18" localSheetId="1">'Formulas OM'!$AA$7</definedName>
-    <definedName name="Dato_18" localSheetId="6">'Formulas PP'!$AA$7</definedName>
-    <definedName name="Dato_18" localSheetId="5">'Formulas RC'!$AA$7</definedName>
-    <definedName name="Dato_18" localSheetId="3">'Formulas VF'!$AA$7</definedName>
-    <definedName name="Dato_19" localSheetId="8">'Formulas CL'!$AA$9</definedName>
-    <definedName name="Dato_19" localSheetId="0">'Formulas DG'!$AA$9</definedName>
-    <definedName name="Dato_19" localSheetId="4">'Formulas EM'!$AA$9</definedName>
-    <definedName name="Dato_19" localSheetId="7">'Formulas EN'!$AA$9</definedName>
-    <definedName name="Dato_19" localSheetId="2">'Formulas O2'!$AA$9</definedName>
-    <definedName name="Dato_19" localSheetId="1">'Formulas OM'!$AA$9</definedName>
-    <definedName name="Dato_19" localSheetId="6">'Formulas PP'!$AA$9</definedName>
-    <definedName name="Dato_19" localSheetId="5">'Formulas RC'!$AA$9</definedName>
-    <definedName name="Dato_19" localSheetId="3">'Formulas VF'!$AA$9</definedName>
-    <definedName name="Dato_20" localSheetId="8">'Formulas CL'!$AA$11</definedName>
-    <definedName name="Dato_20" localSheetId="0">'Formulas DG'!$AA$11</definedName>
-    <definedName name="Dato_20" localSheetId="4">'Formulas EM'!$AA$11</definedName>
-    <definedName name="Dato_20" localSheetId="7">'Formulas EN'!$AA$11</definedName>
-    <definedName name="Dato_20" localSheetId="2">'Formulas O2'!$AA$11</definedName>
-    <definedName name="Dato_20" localSheetId="1">'Formulas OM'!$AA$11</definedName>
-    <definedName name="Dato_20" localSheetId="6">'Formulas PP'!$AA$11</definedName>
-    <definedName name="Dato_20" localSheetId="5">'Formulas RC'!$AA$11</definedName>
-    <definedName name="Dato_20" localSheetId="3">'Formulas VF'!$AA$11</definedName>
-    <definedName name="Dato_21" localSheetId="8">'Formulas CL'!$AA$13</definedName>
-    <definedName name="Dato_21" localSheetId="0">'Formulas DG'!$AA$13</definedName>
-    <definedName name="Dato_21" localSheetId="4">'Formulas EM'!$AA$13</definedName>
-    <definedName name="Dato_21" localSheetId="7">'Formulas EN'!$AA$13</definedName>
-    <definedName name="Dato_21" localSheetId="2">'Formulas O2'!$AA$13</definedName>
-    <definedName name="Dato_21" localSheetId="1">'Formulas OM'!$AA$13</definedName>
-    <definedName name="Dato_21" localSheetId="6">'Formulas PP'!$AA$13</definedName>
-    <definedName name="Dato_21" localSheetId="5">'Formulas RC'!$AA$13</definedName>
-    <definedName name="Dato_21" localSheetId="3">'Formulas VF'!$AA$13</definedName>
-    <definedName name="Dato_22" localSheetId="8">'Formulas CL'!$AA$15</definedName>
-    <definedName name="Dato_22" localSheetId="0">'Formulas DG'!$AA$15</definedName>
-    <definedName name="Dato_22" localSheetId="4">'Formulas EM'!$AA$15</definedName>
-    <definedName name="Dato_22" localSheetId="7">'Formulas EN'!$AA$15</definedName>
-    <definedName name="Dato_22" localSheetId="2">'Formulas O2'!$AA$15</definedName>
-    <definedName name="Dato_22" localSheetId="1">'Formulas OM'!$AA$15</definedName>
-    <definedName name="Dato_22" localSheetId="6">'Formulas PP'!$AA$15</definedName>
-    <definedName name="Dato_22" localSheetId="5">'Formulas RC'!$AA$15</definedName>
-    <definedName name="Dato_22" localSheetId="3">'Formulas VF'!$AA$15</definedName>
-    <definedName name="Dato_23" localSheetId="8">'Formulas CL'!$AA$17</definedName>
-    <definedName name="Dato_23" localSheetId="0">'Formulas DG'!$AA$17</definedName>
-    <definedName name="Dato_23" localSheetId="4">'Formulas EM'!$AA$17</definedName>
-    <definedName name="Dato_23" localSheetId="7">'Formulas EN'!$AA$17</definedName>
-    <definedName name="Dato_23" localSheetId="2">'Formulas O2'!$AA$17</definedName>
-    <definedName name="Dato_23" localSheetId="1">'Formulas OM'!$AA$17</definedName>
-    <definedName name="Dato_23" localSheetId="6">'Formulas PP'!$AA$17</definedName>
-    <definedName name="Dato_23" localSheetId="5">'Formulas RC'!$AA$17</definedName>
-    <definedName name="Dato_23" localSheetId="3">'Formulas VF'!$AA$17</definedName>
-    <definedName name="Dato_24" localSheetId="8">'Formulas CL'!$AA$19</definedName>
-    <definedName name="Dato_24" localSheetId="0">'Formulas DG'!$AA$19</definedName>
-    <definedName name="Dato_24" localSheetId="4">'Formulas EM'!$AA$19</definedName>
-    <definedName name="Dato_24" localSheetId="7">'Formulas EN'!$AA$19</definedName>
-    <definedName name="Dato_24" localSheetId="2">'Formulas O2'!$AA$19</definedName>
-    <definedName name="Dato_24" localSheetId="1">'Formulas OM'!$AA$19</definedName>
-    <definedName name="Dato_24" localSheetId="6">'Formulas PP'!$AA$19</definedName>
-    <definedName name="Dato_24" localSheetId="5">'Formulas RC'!$AA$19</definedName>
-    <definedName name="Dato_24" localSheetId="3">'Formulas VF'!$AA$19</definedName>
-    <definedName name="Dato_25" localSheetId="8">'Formulas CL'!$AA$21</definedName>
-    <definedName name="Dato_25" localSheetId="0">'Formulas DG'!$AA$21</definedName>
-    <definedName name="Dato_25" localSheetId="4">'Formulas EM'!$AA$21</definedName>
-    <definedName name="Dato_25" localSheetId="7">'Formulas EN'!$AA$21</definedName>
-    <definedName name="Dato_25" localSheetId="2">'Formulas O2'!$AA$21</definedName>
-    <definedName name="Dato_25" localSheetId="1">'Formulas OM'!$AA$21</definedName>
-    <definedName name="Dato_25" localSheetId="6">'Formulas PP'!$AA$21</definedName>
-    <definedName name="Dato_25" localSheetId="5">'Formulas RC'!$AA$21</definedName>
-    <definedName name="Dato_25" localSheetId="3">'Formulas VF'!$AA$21</definedName>
-    <definedName name="Dato_26" localSheetId="8">'Formulas CL'!$AA$23</definedName>
-    <definedName name="Dato_27" localSheetId="8">'Formulas CL'!$AA$25</definedName>
-    <definedName name="Dato_28" localSheetId="8">'Formulas CL'!$AA$27</definedName>
-    <definedName name="Dato_29" localSheetId="8">'Formulas CL'!$AA$29</definedName>
-    <definedName name="Dato_30" localSheetId="8">'Formulas CL'!$AA$31</definedName>
-    <definedName name="Dato_31" localSheetId="8">'Formulas CL'!$AA$33</definedName>
-    <definedName name="Dato_32" localSheetId="8">'Formulas CL'!$AA$35</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -222,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="167">
   <si>
     <t>DATO_01</t>
   </si>
@@ -722,10 +544,7 @@
     <t>SubCat_12</t>
   </si>
   <si>
-    <t>ANCHO IMAGEN OM</t>
-  </si>
-  <si>
-    <t>V - 7.7</t>
+    <t>V - 8.0</t>
   </si>
 </sst>
 </file>
@@ -1304,109 +1123,59 @@
   <sheetPr codeName="Hoja9"/>
   <dimension ref="A1:AS49"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AS48" sqref="AS48"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="29" ySplit="4" topLeftCell="AD5" activePane="bottomRight" state="frozen"/>
+      <selection activeCell="A4" sqref="A4"/>
+      <selection pane="topRight" activeCell="AD4" sqref="AD4"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
+      <selection pane="bottomRight" activeCell="AD4" sqref="AD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" zeroHeight="1" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="6.703125" customWidth="1"/>
+    <col min="1" max="1" width="6.64453125" customWidth="1"/>
     <col min="2" max="28" width="0" hidden="1" customWidth="1"/>
-    <col min="29" max="29" width="25.703125" style="1" customWidth="1"/>
-    <col min="30" max="30" width="30.703125" style="14" customWidth="1"/>
+    <col min="29" max="29" width="25.64453125" style="1" customWidth="1"/>
+    <col min="30" max="30" width="30.64453125" style="14" customWidth="1"/>
     <col min="31" max="32" width="0" hidden="1" customWidth="1"/>
-    <col min="33" max="33" width="30.703125" style="14" customWidth="1"/>
+    <col min="33" max="33" width="30.64453125" style="14" customWidth="1"/>
     <col min="34" max="35" width="0" hidden="1" customWidth="1"/>
-    <col min="36" max="36" width="30.703125" style="14" customWidth="1"/>
+    <col min="36" max="36" width="30.64453125" style="14" customWidth="1"/>
     <col min="37" max="38" width="0" hidden="1" customWidth="1"/>
-    <col min="39" max="39" width="30.703125" style="14" customWidth="1"/>
+    <col min="39" max="39" width="30.64453125" style="14" customWidth="1"/>
     <col min="40" max="41" width="0" hidden="1" customWidth="1"/>
-    <col min="42" max="42" width="30.703125" style="14" customWidth="1"/>
+    <col min="42" max="42" width="30.64453125" style="14" customWidth="1"/>
     <col min="43" max="44" width="0" hidden="1" customWidth="1"/>
-    <col min="45" max="45" width="30.703125" style="14" customWidth="1"/>
+    <col min="45" max="45" width="30.64453125" style="14" customWidth="1"/>
     <col min="46" max="47" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:45" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.5">
       <c r="AC1"/>
-      <c r="AD1" t="str">
-        <f>IFERROR(HLOOKUP(AD4,$AB$4:AC4,1,0),"OK")</f>
-        <v>OK</v>
-      </c>
-      <c r="AG1" t="str">
-        <f>IFERROR(HLOOKUP(AG4,$AB$4:AF4,1,0),"OK")</f>
-        <v>OK</v>
-      </c>
-      <c r="AJ1" t="str">
-        <f>IFERROR(HLOOKUP(AJ4,$AB$4:AI4,1,0),"OK")</f>
-        <v>OK</v>
-      </c>
-      <c r="AM1" t="str">
-        <f>IFERROR(HLOOKUP(AM4,$AB$4:AL4,1,0),"OK")</f>
-        <v>OK</v>
-      </c>
-      <c r="AP1" t="str">
-        <f>IFERROR(HLOOKUP(AP4,$AB$4:AO4,1,0),"OK")</f>
-        <v>OK</v>
-      </c>
-      <c r="AS1" t="str">
-        <f>IFERROR(HLOOKUP(AS4,$AB$4:AR4,1,0),"OK")</f>
-        <v>OK</v>
-      </c>
+      <c r="AD1"/>
+      <c r="AG1"/>
+      <c r="AJ1"/>
+      <c r="AM1"/>
+      <c r="AP1"/>
+      <c r="AS1"/>
     </row>
     <row r="2" spans="1:45" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.5">
       <c r="AC2"/>
-      <c r="AD2">
-        <f>COUNTA(AD5:AD36)</f>
-        <v>0</v>
-      </c>
-      <c r="AG2">
-        <f>COUNTA(AG5:AG36)</f>
-        <v>0</v>
-      </c>
-      <c r="AJ2">
-        <f>COUNTA(AJ5:AJ36)</f>
-        <v>0</v>
-      </c>
-      <c r="AM2">
-        <f>COUNTA(AM5:AM36)</f>
-        <v>0</v>
-      </c>
-      <c r="AP2">
-        <f>COUNTA(AP5:AP36)</f>
-        <v>0</v>
-      </c>
-      <c r="AS2">
-        <f>COUNTA(AS5:AS36)</f>
-        <v>0</v>
-      </c>
+      <c r="AD2"/>
+      <c r="AG2"/>
+      <c r="AJ2"/>
+      <c r="AM2"/>
+      <c r="AP2"/>
+      <c r="AS2"/>
     </row>
     <row r="3" spans="1:45" ht="15" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="AC3"/>
-      <c r="AD3">
-        <f>COUNTA(AD39:AD79)</f>
-        <v>0</v>
-      </c>
-      <c r="AG3">
-        <f>COUNTA(AG39:AG79)</f>
-        <v>0</v>
-      </c>
-      <c r="AJ3">
-        <f>COUNTA(AJ39:AJ79)</f>
-        <v>0</v>
-      </c>
-      <c r="AM3">
-        <f>COUNTA(AM39:AM79)</f>
-        <v>0</v>
-      </c>
-      <c r="AP3">
-        <f>COUNTA(AP39:AP79)</f>
-        <v>0</v>
-      </c>
-      <c r="AS3">
-        <f>COUNTA(AS39:AS79)</f>
-        <v>0</v>
-      </c>
+      <c r="AD3"/>
+      <c r="AG3"/>
+      <c r="AJ3"/>
+      <c r="AM3"/>
+      <c r="AP3"/>
+      <c r="AS3"/>
     </row>
     <row r="4" spans="1:45" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="5">
@@ -1813,7 +1582,7 @@
     </row>
     <row r="37" spans="1:45" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="16" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="AC37" s="2"/>
       <c r="AD37" s="2"/>
@@ -1948,7 +1717,7 @@
       <c r="AC49" s="1"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="D0MxQGW/CQ04pELlDXpDaZ8nvcW+2hYugC3VG8ZGPol6I/agbqHwOLQW5g3iDcoztHYpUZ5TqX1P4nDtdgx/lw==" saltValue="hksXG2Jm+t6OsuMkWAM03g==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1" autoFilter="0"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="1J2cDk63Umr0HBBFB3mcMiIbbNXbeKf3TFPTwBtI0JJCmNhayq79KC+79ROGlTowjTQQa80exvwi3r59I3J3MQ==" saltValue="SG3J2yvpvwZWCrpyUTvlOw==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1" autoFilter="0"/>
   <mergeCells count="2">
     <mergeCell ref="A5:A20"/>
     <mergeCell ref="A21:A36"/>
@@ -1965,111 +1734,57 @@
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="29" ySplit="1" topLeftCell="AD5" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="AG14" sqref="AG14"/>
-      <selection pane="topRight" activeCell="AG14" sqref="AG14"/>
-      <selection pane="bottomLeft" activeCell="AG14" sqref="AG14"/>
-      <selection pane="bottomRight" activeCell="AD5" sqref="AD5"/>
+      <selection activeCell="AD5" sqref="AD5"/>
+      <selection pane="topRight" activeCell="AD5" sqref="AD5"/>
+      <selection pane="bottomLeft" activeCell="AD5" sqref="AD5"/>
+      <selection pane="bottomRight" activeCell="AD4" sqref="AD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" zeroHeight="1" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="6.703125" customWidth="1"/>
+    <col min="1" max="1" width="6.64453125" customWidth="1"/>
     <col min="2" max="28" width="0" hidden="1" customWidth="1"/>
-    <col min="29" max="29" width="15.703125" style="1" customWidth="1"/>
-    <col min="30" max="30" width="30.703125" style="1" customWidth="1"/>
+    <col min="29" max="29" width="15.64453125" style="1" customWidth="1"/>
+    <col min="30" max="30" width="30.64453125" style="1" customWidth="1"/>
     <col min="31" max="32" width="0" hidden="1" customWidth="1"/>
-    <col min="33" max="33" width="30.703125" style="1" customWidth="1"/>
+    <col min="33" max="33" width="30.64453125" style="1" customWidth="1"/>
     <col min="34" max="35" width="0" hidden="1" customWidth="1"/>
-    <col min="36" max="36" width="30.703125" style="1" customWidth="1"/>
+    <col min="36" max="36" width="30.64453125" style="1" customWidth="1"/>
     <col min="37" max="38" width="0" hidden="1" customWidth="1"/>
-    <col min="39" max="39" width="30.703125" style="1" customWidth="1"/>
+    <col min="39" max="39" width="30.64453125" style="1" customWidth="1"/>
     <col min="40" max="41" width="0" hidden="1" customWidth="1"/>
-    <col min="42" max="42" width="30.703125" style="1" customWidth="1"/>
+    <col min="42" max="42" width="30.64453125" style="1" customWidth="1"/>
     <col min="43" max="44" width="0" hidden="1" customWidth="1"/>
-    <col min="45" max="45" width="30.703125" style="1" customWidth="1"/>
+    <col min="45" max="45" width="30.64453125" style="1" customWidth="1"/>
     <col min="46" max="47" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:45" x14ac:dyDescent="0.5">
       <c r="AC1"/>
-      <c r="AD1" t="str">
-        <f>IFERROR(HLOOKUP(AD4,$AB$4:AC4,1,0),"OK")</f>
-        <v>OK</v>
-      </c>
-      <c r="AG1" t="str">
-        <f>IFERROR(HLOOKUP(AG4,$AB$4:AF4,1,0),"OK")</f>
-        <v>OK</v>
-      </c>
-      <c r="AJ1" t="str">
-        <f>IFERROR(HLOOKUP(AJ4,$AB$4:AI4,1,0),"OK")</f>
-        <v>OK</v>
-      </c>
-      <c r="AM1" t="str">
-        <f>IFERROR(HLOOKUP(AM4,$AB$4:AL4,1,0),"OK")</f>
-        <v>OK</v>
-      </c>
-      <c r="AP1" t="str">
-        <f>IFERROR(HLOOKUP(AP4,$AB$4:AO4,1,0),"OK")</f>
-        <v>OK</v>
-      </c>
-      <c r="AS1" t="str">
-        <f>IFERROR(HLOOKUP(AS4,$AB$4:AR4,1,0),"OK")</f>
-        <v>OK</v>
-      </c>
+      <c r="AD1"/>
+      <c r="AG1"/>
+      <c r="AJ1"/>
+      <c r="AM1"/>
+      <c r="AP1"/>
+      <c r="AS1"/>
     </row>
     <row r="2" spans="1:45" x14ac:dyDescent="0.5">
       <c r="AC2"/>
-      <c r="AD2">
-        <f>COUNTA(AD5:AD36)</f>
-        <v>0</v>
-      </c>
-      <c r="AG2">
-        <f>COUNTA(AG5:AG36)</f>
-        <v>0</v>
-      </c>
-      <c r="AJ2">
-        <f>COUNTA(AJ5:AJ36)</f>
-        <v>0</v>
-      </c>
-      <c r="AM2">
-        <f>COUNTA(AM5:AM36)</f>
-        <v>0</v>
-      </c>
-      <c r="AP2">
-        <f>COUNTA(AP5:AP36)</f>
-        <v>0</v>
-      </c>
-      <c r="AS2">
-        <f>COUNTA(AS5:AS36)</f>
-        <v>0</v>
-      </c>
+      <c r="AD2"/>
+      <c r="AG2"/>
+      <c r="AJ2"/>
+      <c r="AM2"/>
+      <c r="AP2"/>
+      <c r="AS2"/>
     </row>
     <row r="3" spans="1:45" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="AC3"/>
-      <c r="AD3">
-        <f>COUNTA(AD39:AD79)</f>
-        <v>0</v>
-      </c>
-      <c r="AG3">
-        <f>COUNTA(AG39:AG79)</f>
-        <v>0</v>
-      </c>
-      <c r="AJ3">
-        <f>COUNTA(AJ39:AJ79)</f>
-        <v>0</v>
-      </c>
-      <c r="AM3">
-        <f>COUNTA(AM39:AM79)</f>
-        <v>0</v>
-      </c>
-      <c r="AP3">
-        <f>COUNTA(AP39:AP79)</f>
-        <v>0</v>
-      </c>
-      <c r="AS3">
-        <f>COUNTA(AS39:AS79)</f>
-        <v>0</v>
-      </c>
+      <c r="AD3"/>
+      <c r="AG3"/>
+      <c r="AJ3"/>
+      <c r="AM3"/>
+      <c r="AP3"/>
+      <c r="AS3"/>
     </row>
     <row r="4" spans="1:45" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="5">
@@ -2477,7 +2192,7 @@
     <row r="37" spans="1:45" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="16" t="str">
         <f>'Formulas DG'!A37</f>
-        <v>V - 7.7</v>
+        <v>V - 8.0</v>
       </c>
       <c r="AC37" s="2"/>
       <c r="AD37" s="2"/>
@@ -2775,7 +2490,7 @@
     </row>
     <row r="64" spans="29:45" x14ac:dyDescent="0.5"/>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="XuoGYfeIXLcvT3LgSL8+DXYQZ3T6vKW+M9epkikHtyIpt7HjxdTYFx9ZUouhWIFdv2fKbbAV3da9dXmUG6NPJQ==" saltValue="aHNJL4NCQNEojw9bF+T1PA==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1" autoFilter="0"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="INetjJZjJf24HnHpzIv8W9mpR8VfVSUNKIA4QuN6LoXwwSQkiaHacSKHOrupKeTUxMyeCUnd6D3XmCzQcjWcGg==" saltValue="71kHFML3FQZfN/Hl6ioaQw==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1" autoFilter="0"/>
   <mergeCells count="2">
     <mergeCell ref="A5:A20"/>
     <mergeCell ref="A21:A36"/>
@@ -2792,111 +2507,57 @@
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="29" ySplit="1" topLeftCell="AD5" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="AG14" sqref="AG14"/>
-      <selection pane="topRight" activeCell="AG14" sqref="AG14"/>
-      <selection pane="bottomLeft" activeCell="AG14" sqref="AG14"/>
-      <selection pane="bottomRight" activeCell="AD5" sqref="AD5"/>
+      <selection activeCell="AD5" sqref="AD5"/>
+      <selection pane="topRight" activeCell="AD5" sqref="AD5"/>
+      <selection pane="bottomLeft" activeCell="AD5" sqref="AD5"/>
+      <selection pane="bottomRight" activeCell="AD4" sqref="AD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" zeroHeight="1" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="6.703125" customWidth="1"/>
+    <col min="1" max="1" width="6.64453125" customWidth="1"/>
     <col min="2" max="28" width="0" hidden="1" customWidth="1"/>
-    <col min="29" max="29" width="15.703125" style="1" customWidth="1"/>
-    <col min="30" max="30" width="30.703125" style="1" customWidth="1"/>
+    <col min="29" max="29" width="15.64453125" style="1" customWidth="1"/>
+    <col min="30" max="30" width="30.64453125" style="1" customWidth="1"/>
     <col min="31" max="32" width="0" hidden="1" customWidth="1"/>
-    <col min="33" max="33" width="30.703125" style="1" customWidth="1"/>
+    <col min="33" max="33" width="30.64453125" style="1" customWidth="1"/>
     <col min="34" max="35" width="0" hidden="1" customWidth="1"/>
-    <col min="36" max="36" width="30.703125" style="1" customWidth="1"/>
+    <col min="36" max="36" width="30.64453125" style="1" customWidth="1"/>
     <col min="37" max="38" width="0" hidden="1" customWidth="1"/>
-    <col min="39" max="39" width="30.703125" style="1" customWidth="1"/>
+    <col min="39" max="39" width="30.64453125" style="1" customWidth="1"/>
     <col min="40" max="41" width="0" hidden="1" customWidth="1"/>
-    <col min="42" max="42" width="30.703125" style="1" customWidth="1"/>
+    <col min="42" max="42" width="30.64453125" style="1" customWidth="1"/>
     <col min="43" max="44" width="0" hidden="1" customWidth="1"/>
-    <col min="45" max="45" width="30.703125" style="1" customWidth="1"/>
+    <col min="45" max="45" width="30.64453125" style="1" customWidth="1"/>
     <col min="46" max="47" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:45" x14ac:dyDescent="0.5">
       <c r="AC1"/>
-      <c r="AD1" t="str">
-        <f>IFERROR(HLOOKUP(AD4,$AB$4:AC4,1,0),"OK")</f>
-        <v>OK</v>
-      </c>
-      <c r="AG1" t="str">
-        <f>IFERROR(HLOOKUP(AG4,$AB$4:AF4,1,0),"OK")</f>
-        <v>OK</v>
-      </c>
-      <c r="AJ1" t="str">
-        <f>IFERROR(HLOOKUP(AJ4,$AB$4:AI4,1,0),"OK")</f>
-        <v>OK</v>
-      </c>
-      <c r="AM1" t="str">
-        <f>IFERROR(HLOOKUP(AM4,$AB$4:AL4,1,0),"OK")</f>
-        <v>OK</v>
-      </c>
-      <c r="AP1" t="str">
-        <f>IFERROR(HLOOKUP(AP4,$AB$4:AO4,1,0),"OK")</f>
-        <v>OK</v>
-      </c>
-      <c r="AS1" t="str">
-        <f>IFERROR(HLOOKUP(AS4,$AB$4:AR4,1,0),"OK")</f>
-        <v>OK</v>
-      </c>
+      <c r="AD1"/>
+      <c r="AG1"/>
+      <c r="AJ1"/>
+      <c r="AM1"/>
+      <c r="AP1"/>
+      <c r="AS1"/>
     </row>
     <row r="2" spans="1:45" x14ac:dyDescent="0.5">
       <c r="AC2"/>
-      <c r="AD2">
-        <f>COUNTA(AD5:AD36)</f>
-        <v>0</v>
-      </c>
-      <c r="AG2">
-        <f>COUNTA(AG5:AG36)</f>
-        <v>0</v>
-      </c>
-      <c r="AJ2">
-        <f>COUNTA(AJ5:AJ36)</f>
-        <v>0</v>
-      </c>
-      <c r="AM2">
-        <f>COUNTA(AM5:AM36)</f>
-        <v>0</v>
-      </c>
-      <c r="AP2">
-        <f>COUNTA(AP5:AP36)</f>
-        <v>0</v>
-      </c>
-      <c r="AS2">
-        <f>COUNTA(AS5:AS36)</f>
-        <v>0</v>
-      </c>
+      <c r="AD2"/>
+      <c r="AG2"/>
+      <c r="AJ2"/>
+      <c r="AM2"/>
+      <c r="AP2"/>
+      <c r="AS2"/>
     </row>
     <row r="3" spans="1:45" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="AC3"/>
-      <c r="AD3">
-        <f>COUNTA(AD39:AD79)</f>
-        <v>0</v>
-      </c>
-      <c r="AG3">
-        <f>COUNTA(AG39:AG79)</f>
-        <v>0</v>
-      </c>
-      <c r="AJ3">
-        <f>COUNTA(AJ39:AJ79)</f>
-        <v>0</v>
-      </c>
-      <c r="AM3">
-        <f>COUNTA(AM39:AM79)</f>
-        <v>0</v>
-      </c>
-      <c r="AP3">
-        <f>COUNTA(AP39:AP79)</f>
-        <v>0</v>
-      </c>
-      <c r="AS3">
-        <f>COUNTA(AS39:AS79)</f>
-        <v>0</v>
-      </c>
+      <c r="AD3"/>
+      <c r="AG3"/>
+      <c r="AJ3"/>
+      <c r="AM3"/>
+      <c r="AP3"/>
+      <c r="AS3"/>
     </row>
     <row r="4" spans="1:45" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="5">
@@ -3304,7 +2965,7 @@
     <row r="37" spans="1:45" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="16" t="str">
         <f>'Formulas OM'!A37</f>
-        <v>V - 7.7</v>
+        <v>V - 8.0</v>
       </c>
       <c r="AC37" s="2"/>
       <c r="AD37" s="2"/>
@@ -3602,7 +3263,7 @@
     </row>
     <row r="64" spans="29:45" x14ac:dyDescent="0.5"/>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="sIxvDV7giMTM0O4LJxC+KCNi0/CCZDtQ/Yh8WL72fd8MiTkPMpauSj+EVki5HC8pGeSTgKt4n5dG+hhTkFRvOQ==" saltValue="iuMvsB3eU8AOrlqUhkNaoA==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1" autoFilter="0"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="+mQxza9Wp3g6U8YISAvfazW79LwEi3cBb7iDssIwVBag/ECl6GDuNW7emvJMfBAziSf7q86+TzhCI8s3TDRT9Q==" saltValue="hRIpu6dqldriMXfqAJgKCQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1" autoFilter="0"/>
   <mergeCells count="2">
     <mergeCell ref="A5:A20"/>
     <mergeCell ref="A21:A36"/>
@@ -3618,111 +3279,57 @@
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="29" ySplit="1" topLeftCell="AD5" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="AG14" sqref="AG14"/>
-      <selection pane="topRight" activeCell="AG14" sqref="AG14"/>
-      <selection pane="bottomLeft" activeCell="AG14" sqref="AG14"/>
-      <selection pane="bottomRight" activeCell="AD5" sqref="AD5"/>
+      <selection activeCell="AD5" sqref="AD5"/>
+      <selection pane="topRight" activeCell="AD5" sqref="AD5"/>
+      <selection pane="bottomLeft" activeCell="AD5" sqref="AD5"/>
+      <selection pane="bottomRight" activeCell="AD4" sqref="AD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" zeroHeight="1" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="6.703125" customWidth="1"/>
+    <col min="1" max="1" width="6.64453125" customWidth="1"/>
     <col min="2" max="28" width="0" hidden="1" customWidth="1"/>
-    <col min="29" max="29" width="15.703125" style="1" customWidth="1"/>
-    <col min="30" max="30" width="30.703125" style="14" customWidth="1"/>
+    <col min="29" max="29" width="15.64453125" style="1" customWidth="1"/>
+    <col min="30" max="30" width="30.64453125" style="14" customWidth="1"/>
     <col min="31" max="32" width="0" hidden="1" customWidth="1"/>
-    <col min="33" max="33" width="30.703125" style="14" customWidth="1"/>
+    <col min="33" max="33" width="30.64453125" style="14" customWidth="1"/>
     <col min="34" max="35" width="0" hidden="1" customWidth="1"/>
-    <col min="36" max="36" width="30.703125" style="14" customWidth="1"/>
+    <col min="36" max="36" width="30.64453125" style="14" customWidth="1"/>
     <col min="37" max="38" width="0" hidden="1" customWidth="1"/>
-    <col min="39" max="39" width="30.703125" style="14" customWidth="1"/>
+    <col min="39" max="39" width="30.64453125" style="14" customWidth="1"/>
     <col min="40" max="41" width="0" hidden="1" customWidth="1"/>
-    <col min="42" max="42" width="30.703125" style="14" customWidth="1"/>
+    <col min="42" max="42" width="30.64453125" style="14" customWidth="1"/>
     <col min="43" max="44" width="0" hidden="1" customWidth="1"/>
-    <col min="45" max="45" width="30.703125" style="14" customWidth="1"/>
+    <col min="45" max="45" width="30.64453125" style="14" customWidth="1"/>
     <col min="46" max="47" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:45" x14ac:dyDescent="0.5">
       <c r="AC1"/>
-      <c r="AD1" t="str">
-        <f>IFERROR(HLOOKUP(AD4,$AB$4:AC4,1,0),"OK")</f>
-        <v>OK</v>
-      </c>
-      <c r="AG1" t="str">
-        <f>IFERROR(HLOOKUP(AG4,$AB$4:AF4,1,0),"OK")</f>
-        <v>OK</v>
-      </c>
-      <c r="AJ1" t="str">
-        <f>IFERROR(HLOOKUP(AJ4,$AB$4:AI4,1,0),"OK")</f>
-        <v>OK</v>
-      </c>
-      <c r="AM1" t="str">
-        <f>IFERROR(HLOOKUP(AM4,$AB$4:AL4,1,0),"OK")</f>
-        <v>OK</v>
-      </c>
-      <c r="AP1" t="str">
-        <f>IFERROR(HLOOKUP(AP4,$AB$4:AO4,1,0),"OK")</f>
-        <v>OK</v>
-      </c>
-      <c r="AS1" t="str">
-        <f>IFERROR(HLOOKUP(AS4,$AB$4:AR4,1,0),"OK")</f>
-        <v>OK</v>
-      </c>
+      <c r="AD1"/>
+      <c r="AG1"/>
+      <c r="AJ1"/>
+      <c r="AM1"/>
+      <c r="AP1"/>
+      <c r="AS1"/>
     </row>
     <row r="2" spans="1:45" x14ac:dyDescent="0.5">
       <c r="AC2"/>
-      <c r="AD2">
-        <f>COUNTA(AD5:AD36)</f>
-        <v>0</v>
-      </c>
-      <c r="AG2">
-        <f>COUNTA(AG5:AG36)</f>
-        <v>0</v>
-      </c>
-      <c r="AJ2">
-        <f>COUNTA(AJ5:AJ36)</f>
-        <v>0</v>
-      </c>
-      <c r="AM2">
-        <f>COUNTA(AM5:AM36)</f>
-        <v>0</v>
-      </c>
-      <c r="AP2">
-        <f>COUNTA(AP5:AP36)</f>
-        <v>0</v>
-      </c>
-      <c r="AS2">
-        <f>COUNTA(AS5:AS36)</f>
-        <v>0</v>
-      </c>
+      <c r="AD2"/>
+      <c r="AG2"/>
+      <c r="AJ2"/>
+      <c r="AM2"/>
+      <c r="AP2"/>
+      <c r="AS2"/>
     </row>
     <row r="3" spans="1:45" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="AC3"/>
-      <c r="AD3">
-        <f>COUNTA(AD39:AD79)</f>
-        <v>0</v>
-      </c>
-      <c r="AG3">
-        <f>COUNTA(AG39:AG79)</f>
-        <v>0</v>
-      </c>
-      <c r="AJ3">
-        <f>COUNTA(AJ39:AJ79)</f>
-        <v>0</v>
-      </c>
-      <c r="AM3">
-        <f>COUNTA(AM39:AM79)</f>
-        <v>0</v>
-      </c>
-      <c r="AP3">
-        <f>COUNTA(AP39:AP79)</f>
-        <v>0</v>
-      </c>
-      <c r="AS3">
-        <f>COUNTA(AS39:AS79)</f>
-        <v>0</v>
-      </c>
+      <c r="AD3"/>
+      <c r="AG3"/>
+      <c r="AJ3"/>
+      <c r="AM3"/>
+      <c r="AP3"/>
+      <c r="AS3"/>
     </row>
     <row r="4" spans="1:45" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="5">
@@ -4130,7 +3737,7 @@
     <row r="37" spans="1:45" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="16" t="str">
         <f>'Formulas OM'!A37</f>
-        <v>V - 7.7</v>
+        <v>V - 8.0</v>
       </c>
       <c r="AC37" s="2"/>
       <c r="AD37" s="2"/>
@@ -4275,7 +3882,7 @@
       <c r="AC49" s="1"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="rFsbKTcon+fBMQokExHj58MF/fJnK6qs/19JFsnMNtkStcom0SbdkP2aq6ggByjMt58mCbm6I/Fpu9BxIIQpdA==" saltValue="tjDt5WluSJpWzEyWFStjEg==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1" autoFilter="0"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="kl5FXaR4QE2lOSA8h8WkH4h4zLH1QH3/abfnprYXtfC170ag7NtuwYYykb/o6tWKCPHzLnPzVJVxVoxkUzw3Mw==" saltValue="f7sdpnT901ndWLN8uAP93A==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1" autoFilter="0"/>
   <mergeCells count="2">
     <mergeCell ref="A5:A20"/>
     <mergeCell ref="A21:A36"/>
@@ -4292,111 +3899,57 @@
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="29" ySplit="1" topLeftCell="AD5" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="AG14" sqref="AG14"/>
-      <selection pane="topRight" activeCell="AG14" sqref="AG14"/>
-      <selection pane="bottomLeft" activeCell="AG14" sqref="AG14"/>
-      <selection pane="bottomRight" activeCell="AD5" sqref="AD5"/>
+      <selection activeCell="AD5" sqref="AD5"/>
+      <selection pane="topRight" activeCell="AD5" sqref="AD5"/>
+      <selection pane="bottomLeft" activeCell="AD5" sqref="AD5"/>
+      <selection pane="bottomRight" activeCell="AD4" sqref="AD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" zeroHeight="1" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="6.703125" customWidth="1"/>
+    <col min="1" max="1" width="6.64453125" customWidth="1"/>
     <col min="2" max="28" width="0" hidden="1" customWidth="1"/>
-    <col min="29" max="29" width="15.703125" style="1" customWidth="1"/>
-    <col min="30" max="30" width="30.703125" style="1" customWidth="1"/>
+    <col min="29" max="29" width="15.64453125" style="1" customWidth="1"/>
+    <col min="30" max="30" width="30.64453125" style="1" customWidth="1"/>
     <col min="31" max="32" width="0" hidden="1" customWidth="1"/>
-    <col min="33" max="33" width="30.703125" style="1" customWidth="1"/>
+    <col min="33" max="33" width="30.64453125" style="1" customWidth="1"/>
     <col min="34" max="35" width="0" hidden="1" customWidth="1"/>
-    <col min="36" max="36" width="30.703125" style="1" customWidth="1"/>
+    <col min="36" max="36" width="30.64453125" style="1" customWidth="1"/>
     <col min="37" max="38" width="0" hidden="1" customWidth="1"/>
-    <col min="39" max="39" width="30.703125" style="1" customWidth="1"/>
+    <col min="39" max="39" width="30.64453125" style="1" customWidth="1"/>
     <col min="40" max="41" width="0" hidden="1" customWidth="1"/>
-    <col min="42" max="42" width="30.703125" style="1" customWidth="1"/>
+    <col min="42" max="42" width="30.64453125" style="1" customWidth="1"/>
     <col min="43" max="44" width="0" hidden="1" customWidth="1"/>
-    <col min="45" max="45" width="30.703125" style="1" customWidth="1"/>
+    <col min="45" max="45" width="30.64453125" style="1" customWidth="1"/>
     <col min="46" max="47" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:45" x14ac:dyDescent="0.5">
       <c r="AC1"/>
-      <c r="AD1" t="str">
-        <f>IFERROR(HLOOKUP(AD4,$AB$4:AC4,1,0),"OK")</f>
-        <v>OK</v>
-      </c>
-      <c r="AG1" t="str">
-        <f>IFERROR(HLOOKUP(AG4,$AB$4:AF4,1,0),"OK")</f>
-        <v>OK</v>
-      </c>
-      <c r="AJ1" t="str">
-        <f>IFERROR(HLOOKUP(AJ4,$AB$4:AI4,1,0),"OK")</f>
-        <v>OK</v>
-      </c>
-      <c r="AM1" t="str">
-        <f>IFERROR(HLOOKUP(AM4,$AB$4:AL4,1,0),"OK")</f>
-        <v>OK</v>
-      </c>
-      <c r="AP1" t="str">
-        <f>IFERROR(HLOOKUP(AP4,$AB$4:AO4,1,0),"OK")</f>
-        <v>OK</v>
-      </c>
-      <c r="AS1" t="str">
-        <f>IFERROR(HLOOKUP(AS4,$AB$4:AR4,1,0),"OK")</f>
-        <v>OK</v>
-      </c>
+      <c r="AD1"/>
+      <c r="AG1"/>
+      <c r="AJ1"/>
+      <c r="AM1"/>
+      <c r="AP1"/>
+      <c r="AS1"/>
     </row>
     <row r="2" spans="1:45" x14ac:dyDescent="0.5">
       <c r="AC2"/>
-      <c r="AD2">
-        <f>COUNTA(AD5:AD36)</f>
-        <v>0</v>
-      </c>
-      <c r="AG2">
-        <f>COUNTA(AG5:AG36)</f>
-        <v>0</v>
-      </c>
-      <c r="AJ2">
-        <f>COUNTA(AJ5:AJ36)</f>
-        <v>0</v>
-      </c>
-      <c r="AM2">
-        <f>COUNTA(AM5:AM36)</f>
-        <v>0</v>
-      </c>
-      <c r="AP2">
-        <f>COUNTA(AP5:AP36)</f>
-        <v>0</v>
-      </c>
-      <c r="AS2">
-        <f>COUNTA(AS5:AS36)</f>
-        <v>0</v>
-      </c>
+      <c r="AD2"/>
+      <c r="AG2"/>
+      <c r="AJ2"/>
+      <c r="AM2"/>
+      <c r="AP2"/>
+      <c r="AS2"/>
     </row>
     <row r="3" spans="1:45" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="AC3"/>
-      <c r="AD3">
-        <f>COUNTA(AD39:AD79)</f>
-        <v>0</v>
-      </c>
-      <c r="AG3">
-        <f>COUNTA(AG39:AG79)</f>
-        <v>0</v>
-      </c>
-      <c r="AJ3">
-        <f>COUNTA(AJ39:AJ79)</f>
-        <v>0</v>
-      </c>
-      <c r="AM3">
-        <f>COUNTA(AM39:AM79)</f>
-        <v>0</v>
-      </c>
-      <c r="AP3">
-        <f>COUNTA(AP39:AP79)</f>
-        <v>0</v>
-      </c>
-      <c r="AS3">
-        <f>COUNTA(AS39:AS79)</f>
-        <v>0</v>
-      </c>
+      <c r="AD3"/>
+      <c r="AG3"/>
+      <c r="AJ3"/>
+      <c r="AM3"/>
+      <c r="AP3"/>
+      <c r="AS3"/>
     </row>
     <row r="4" spans="1:45" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="5">
@@ -4804,7 +4357,7 @@
     <row r="37" spans="1:45" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="16" t="str">
         <f>'Formulas OM'!A37</f>
-        <v>V - 7.7</v>
+        <v>V - 8.0</v>
       </c>
       <c r="AC37" s="2"/>
       <c r="AD37" s="2"/>
@@ -5168,7 +4721,7 @@
     </row>
     <row r="70" spans="29:45" x14ac:dyDescent="0.5"/>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="fTmXKp1BtdDjqox0lnBFBP4w0+uozF4Ht93RP6PWfi226a3WcEfnWy12hVI80iP8ufXmQWhOhhIZrQEanAf8Yw==" saltValue="QH0ae+8WZyxk6+g4kEu62w==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1" autoFilter="0"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="tAZ6UCeLSW4DUrSeHGdEb12uNpcFxUP2PjcIQkUyGWwJZ4VbPHk3i5qr9WYbnpkXO0uXiB8ee8uLj7wKxdqKFw==" saltValue="g5kttvYrX/uTE9ctJRRVrw==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1" autoFilter="0"/>
   <mergeCells count="2">
     <mergeCell ref="A5:A20"/>
     <mergeCell ref="A21:A36"/>
@@ -5184,111 +4737,57 @@
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="29" ySplit="1" topLeftCell="AD5" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="AG14" sqref="AG14"/>
-      <selection pane="topRight" activeCell="AG14" sqref="AG14"/>
-      <selection pane="bottomLeft" activeCell="AG14" sqref="AG14"/>
-      <selection pane="bottomRight" activeCell="AD5" sqref="AD5"/>
+      <selection activeCell="AD5" sqref="AD5"/>
+      <selection pane="topRight" activeCell="AD5" sqref="AD5"/>
+      <selection pane="bottomLeft" activeCell="AD5" sqref="AD5"/>
+      <selection pane="bottomRight" activeCell="AD4" sqref="AD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" zeroHeight="1" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="6.703125" customWidth="1"/>
+    <col min="1" max="1" width="6.64453125" customWidth="1"/>
     <col min="2" max="28" width="0" hidden="1" customWidth="1"/>
-    <col min="29" max="29" width="15.703125" style="1" customWidth="1"/>
-    <col min="30" max="30" width="30.703125" style="1" customWidth="1"/>
+    <col min="29" max="29" width="15.64453125" style="1" customWidth="1"/>
+    <col min="30" max="30" width="30.64453125" style="1" customWidth="1"/>
     <col min="31" max="32" width="0" hidden="1" customWidth="1"/>
-    <col min="33" max="33" width="30.703125" style="1" customWidth="1"/>
+    <col min="33" max="33" width="30.64453125" style="1" customWidth="1"/>
     <col min="34" max="35" width="0" hidden="1" customWidth="1"/>
-    <col min="36" max="36" width="30.703125" style="1" customWidth="1"/>
+    <col min="36" max="36" width="30.64453125" style="1" customWidth="1"/>
     <col min="37" max="38" width="0" hidden="1" customWidth="1"/>
-    <col min="39" max="39" width="30.703125" style="1" customWidth="1"/>
+    <col min="39" max="39" width="30.64453125" style="1" customWidth="1"/>
     <col min="40" max="41" width="0" hidden="1" customWidth="1"/>
-    <col min="42" max="42" width="30.703125" style="1" customWidth="1"/>
+    <col min="42" max="42" width="30.64453125" style="1" customWidth="1"/>
     <col min="43" max="44" width="0" hidden="1" customWidth="1"/>
-    <col min="45" max="45" width="30.703125" style="1" customWidth="1"/>
+    <col min="45" max="45" width="30.64453125" style="1" customWidth="1"/>
     <col min="46" max="47" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:45" x14ac:dyDescent="0.5">
       <c r="AC1"/>
-      <c r="AD1" t="str">
-        <f>IFERROR(HLOOKUP(AD4,$AB$4:AC4,1,0),"OK")</f>
-        <v>OK</v>
-      </c>
-      <c r="AG1" t="str">
-        <f>IFERROR(HLOOKUP(AG4,$AB$4:AF4,1,0),"OK")</f>
-        <v>OK</v>
-      </c>
-      <c r="AJ1" t="str">
-        <f>IFERROR(HLOOKUP(AJ4,$AB$4:AI4,1,0),"OK")</f>
-        <v>OK</v>
-      </c>
-      <c r="AM1" t="str">
-        <f>IFERROR(HLOOKUP(AM4,$AB$4:AL4,1,0),"OK")</f>
-        <v>OK</v>
-      </c>
-      <c r="AP1" t="str">
-        <f>IFERROR(HLOOKUP(AP4,$AB$4:AO4,1,0),"OK")</f>
-        <v>OK</v>
-      </c>
-      <c r="AS1" t="str">
-        <f>IFERROR(HLOOKUP(AS4,$AB$4:AR4,1,0),"OK")</f>
-        <v>OK</v>
-      </c>
+      <c r="AD1"/>
+      <c r="AG1"/>
+      <c r="AJ1"/>
+      <c r="AM1"/>
+      <c r="AP1"/>
+      <c r="AS1"/>
     </row>
     <row r="2" spans="1:45" x14ac:dyDescent="0.5">
       <c r="AC2"/>
-      <c r="AD2">
-        <f>COUNTA(AD5:AD36)</f>
-        <v>0</v>
-      </c>
-      <c r="AG2">
-        <f>COUNTA(AG5:AG36)</f>
-        <v>0</v>
-      </c>
-      <c r="AJ2">
-        <f>COUNTA(AJ5:AJ36)</f>
-        <v>0</v>
-      </c>
-      <c r="AM2">
-        <f>COUNTA(AM5:AM36)</f>
-        <v>0</v>
-      </c>
-      <c r="AP2">
-        <f>COUNTA(AP5:AP36)</f>
-        <v>0</v>
-      </c>
-      <c r="AS2">
-        <f>COUNTA(AS5:AS36)</f>
-        <v>0</v>
-      </c>
+      <c r="AD2"/>
+      <c r="AG2"/>
+      <c r="AJ2"/>
+      <c r="AM2"/>
+      <c r="AP2"/>
+      <c r="AS2"/>
     </row>
     <row r="3" spans="1:45" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="AC3"/>
-      <c r="AD3">
-        <f>COUNTA(AD39:AD79)</f>
-        <v>0</v>
-      </c>
-      <c r="AG3">
-        <f>COUNTA(AG39:AG79)</f>
-        <v>0</v>
-      </c>
-      <c r="AJ3">
-        <f>COUNTA(AJ39:AJ79)</f>
-        <v>0</v>
-      </c>
-      <c r="AM3">
-        <f>COUNTA(AM39:AM79)</f>
-        <v>0</v>
-      </c>
-      <c r="AP3">
-        <f>COUNTA(AP39:AP79)</f>
-        <v>0</v>
-      </c>
-      <c r="AS3">
-        <f>COUNTA(AS39:AS79)</f>
-        <v>0</v>
-      </c>
+      <c r="AD3"/>
+      <c r="AG3"/>
+      <c r="AJ3"/>
+      <c r="AM3"/>
+      <c r="AP3"/>
+      <c r="AS3"/>
     </row>
     <row r="4" spans="1:45" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="5">
@@ -5696,7 +5195,7 @@
     <row r="37" spans="1:45" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="16" t="str">
         <f>'Formulas OM'!A37</f>
-        <v>V - 7.7</v>
+        <v>V - 8.0</v>
       </c>
       <c r="AC37" s="2"/>
       <c r="AD37" s="2"/>
@@ -6079,7 +5578,7 @@
       <c r="AS71"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="Q1uxb3sV3j7tPxeHm3GPWD9xwmOs3oebXRGoWhhrztodu0grWFk1jJPJ9plEIgYoD1ncdCxxramNTs2WRg9WWg==" saltValue="KLT3BejcIHoPVBH3vLnoGA==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1" autoFilter="0"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="mw+DdyguqclqTK4ArGaRpvtQkIcL5yk7lagquQQ3+nHmxBy5qbhjQS2G3cTXMtCWIa9ralfBpCigUJN6Op+F0g==" saltValue="NjRi0jRoEIPtsgMmXEtXBQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1" autoFilter="0"/>
   <mergeCells count="2">
     <mergeCell ref="A5:A20"/>
     <mergeCell ref="A21:A36"/>
@@ -6095,111 +5594,57 @@
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="29" ySplit="1" topLeftCell="AD5" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="AG14" sqref="AG14"/>
-      <selection pane="topRight" activeCell="AG14" sqref="AG14"/>
-      <selection pane="bottomLeft" activeCell="AG14" sqref="AG14"/>
-      <selection pane="bottomRight" activeCell="AD5" sqref="AD5"/>
+      <selection activeCell="AD5" sqref="AD5"/>
+      <selection pane="topRight" activeCell="AD5" sqref="AD5"/>
+      <selection pane="bottomLeft" activeCell="AD5" sqref="AD5"/>
+      <selection pane="bottomRight" activeCell="AD4" sqref="AD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" zeroHeight="1" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="6.703125" customWidth="1"/>
+    <col min="1" max="1" width="6.64453125" customWidth="1"/>
     <col min="2" max="28" width="0" hidden="1" customWidth="1"/>
-    <col min="29" max="29" width="15.703125" style="1" customWidth="1"/>
-    <col min="30" max="30" width="30.703125" style="22" customWidth="1"/>
+    <col min="29" max="29" width="15.64453125" style="1" customWidth="1"/>
+    <col min="30" max="30" width="30.64453125" style="22" customWidth="1"/>
     <col min="31" max="32" width="0" hidden="1" customWidth="1"/>
-    <col min="33" max="33" width="30.703125" style="22" customWidth="1"/>
+    <col min="33" max="33" width="30.64453125" style="22" customWidth="1"/>
     <col min="34" max="35" width="0" hidden="1" customWidth="1"/>
-    <col min="36" max="36" width="30.703125" style="22" customWidth="1"/>
+    <col min="36" max="36" width="30.64453125" style="22" customWidth="1"/>
     <col min="37" max="38" width="0" hidden="1" customWidth="1"/>
-    <col min="39" max="39" width="30.703125" style="22" customWidth="1"/>
+    <col min="39" max="39" width="30.64453125" style="22" customWidth="1"/>
     <col min="40" max="41" width="0" hidden="1" customWidth="1"/>
-    <col min="42" max="42" width="30.703125" style="22" customWidth="1"/>
+    <col min="42" max="42" width="30.64453125" style="22" customWidth="1"/>
     <col min="43" max="44" width="0" hidden="1" customWidth="1"/>
-    <col min="45" max="45" width="30.703125" style="22" customWidth="1"/>
+    <col min="45" max="45" width="30.64453125" style="22" customWidth="1"/>
     <col min="46" max="47" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:45" x14ac:dyDescent="0.5">
       <c r="AC1"/>
-      <c r="AD1" s="14" t="str">
-        <f>IFERROR(HLOOKUP(AD4,$AB$4:AC4,1,0),"OK")</f>
-        <v>OK</v>
-      </c>
-      <c r="AG1" s="14" t="str">
-        <f>IFERROR(HLOOKUP(AG4,$AB$4:AF4,1,0),"OK")</f>
-        <v>OK</v>
-      </c>
-      <c r="AJ1" s="14" t="str">
-        <f>IFERROR(HLOOKUP(AJ4,$AB$4:AI4,1,0),"OK")</f>
-        <v>OK</v>
-      </c>
-      <c r="AM1" s="14" t="str">
-        <f>IFERROR(HLOOKUP(AM4,$AB$4:AL4,1,0),"OK")</f>
-        <v>OK</v>
-      </c>
-      <c r="AP1" s="14" t="str">
-        <f>IFERROR(HLOOKUP(AP4,$AB$4:AO4,1,0),"OK")</f>
-        <v>OK</v>
-      </c>
-      <c r="AS1" s="14" t="str">
-        <f>IFERROR(HLOOKUP(AS4,$AB$4:AR4,1,0),"OK")</f>
-        <v>OK</v>
-      </c>
+      <c r="AD1" s="14"/>
+      <c r="AG1" s="14"/>
+      <c r="AJ1" s="14"/>
+      <c r="AM1" s="14"/>
+      <c r="AP1" s="14"/>
+      <c r="AS1" s="14"/>
     </row>
     <row r="2" spans="1:45" x14ac:dyDescent="0.5">
       <c r="AC2"/>
-      <c r="AD2" s="14">
-        <f>COUNTA(AD5:AD36)</f>
-        <v>0</v>
-      </c>
-      <c r="AG2" s="14">
-        <f>COUNTA(AG5:AG36)</f>
-        <v>0</v>
-      </c>
-      <c r="AJ2" s="14">
-        <f>COUNTA(AJ5:AJ36)</f>
-        <v>0</v>
-      </c>
-      <c r="AM2" s="14">
-        <f>COUNTA(AM5:AM36)</f>
-        <v>0</v>
-      </c>
-      <c r="AP2" s="14">
-        <f>COUNTA(AP5:AP36)</f>
-        <v>0</v>
-      </c>
-      <c r="AS2" s="14">
-        <f>COUNTA(AS5:AS36)</f>
-        <v>0</v>
-      </c>
+      <c r="AD2" s="14"/>
+      <c r="AG2" s="14"/>
+      <c r="AJ2" s="14"/>
+      <c r="AM2" s="14"/>
+      <c r="AP2" s="14"/>
+      <c r="AS2" s="14"/>
     </row>
     <row r="3" spans="1:45" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="AC3"/>
-      <c r="AD3" s="14">
-        <f>COUNTA(AD39:AD79)</f>
-        <v>0</v>
-      </c>
-      <c r="AG3" s="14">
-        <f>COUNTA(AG39:AG79)</f>
-        <v>0</v>
-      </c>
-      <c r="AJ3" s="14">
-        <f>COUNTA(AJ39:AJ79)</f>
-        <v>0</v>
-      </c>
-      <c r="AM3" s="14">
-        <f>COUNTA(AM39:AM79)</f>
-        <v>0</v>
-      </c>
-      <c r="AP3" s="14">
-        <f>COUNTA(AP39:AP79)</f>
-        <v>0</v>
-      </c>
-      <c r="AS3" s="14">
-        <f>COUNTA(AS39:AS79)</f>
-        <v>0</v>
-      </c>
+      <c r="AD3" s="14"/>
+      <c r="AG3" s="14"/>
+      <c r="AJ3" s="14"/>
+      <c r="AM3" s="14"/>
+      <c r="AP3" s="14"/>
+      <c r="AS3" s="14"/>
     </row>
     <row r="4" spans="1:45" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="5">
@@ -6607,7 +6052,7 @@
     <row r="37" spans="1:45" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="16" t="str">
         <f>'Formulas OM'!A37</f>
-        <v>V - 7.7</v>
+        <v>V - 8.0</v>
       </c>
       <c r="AC37" s="2"/>
       <c r="AD37" s="2"/>
@@ -6978,7 +6423,7 @@
       <c r="AS70" s="1"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="xXpAjZoDBthIuKXXenaIFrFD+CMQdAFo7uoXVrKoFNzu1RcY5svj6/4zGQzhdc50boF00sIBbx73dOTbs27Brw==" saltValue="TOcBkZHg7kgPsyRTlMNNdA==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1" autoFilter="0"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="y76TPVc7MNSb8nK/+cTeoe9+D7sWbrSXC4t9wjWj7hS8K4L6Qir3iWAOzgmhxqp1beTdCiBhvQyVDyIiKlgQbw==" saltValue="hXPhg094EVz5P35Wwhq+CA==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1" autoFilter="0"/>
   <mergeCells count="2">
     <mergeCell ref="A5:A20"/>
     <mergeCell ref="A21:A36"/>
@@ -6994,111 +6439,57 @@
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="29" ySplit="4" topLeftCell="AD5" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="AG14" sqref="AG14"/>
-      <selection pane="topRight" activeCell="AG14" sqref="AG14"/>
-      <selection pane="bottomLeft" activeCell="AG14" sqref="AG14"/>
-      <selection pane="bottomRight" activeCell="AD5" sqref="AD5"/>
+      <selection activeCell="AD5" sqref="AD5"/>
+      <selection pane="topRight" activeCell="AD5" sqref="AD5"/>
+      <selection pane="bottomLeft" activeCell="AD5" sqref="AD5"/>
+      <selection pane="bottomRight" activeCell="AD4" sqref="AD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" zeroHeight="1" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="6.703125" customWidth="1"/>
+    <col min="1" max="1" width="6.64453125" customWidth="1"/>
     <col min="2" max="28" width="0" hidden="1" customWidth="1"/>
-    <col min="29" max="29" width="15.703125" style="1" customWidth="1"/>
-    <col min="30" max="30" width="30.703125" style="14" customWidth="1"/>
+    <col min="29" max="29" width="15.64453125" style="1" customWidth="1"/>
+    <col min="30" max="30" width="30.64453125" style="14" customWidth="1"/>
     <col min="31" max="32" width="0" hidden="1" customWidth="1"/>
-    <col min="33" max="33" width="30.703125" style="14" customWidth="1"/>
+    <col min="33" max="33" width="30.64453125" style="14" customWidth="1"/>
     <col min="34" max="35" width="0" hidden="1" customWidth="1"/>
-    <col min="36" max="36" width="30.703125" style="14" customWidth="1"/>
+    <col min="36" max="36" width="30.64453125" style="14" customWidth="1"/>
     <col min="37" max="38" width="0" hidden="1" customWidth="1"/>
-    <col min="39" max="39" width="30.703125" style="14" customWidth="1"/>
+    <col min="39" max="39" width="30.64453125" style="14" customWidth="1"/>
     <col min="40" max="41" width="0" hidden="1" customWidth="1"/>
-    <col min="42" max="42" width="30.703125" style="14" customWidth="1"/>
+    <col min="42" max="42" width="30.64453125" style="14" customWidth="1"/>
     <col min="43" max="44" width="0" hidden="1" customWidth="1"/>
-    <col min="45" max="45" width="30.703125" style="14" customWidth="1"/>
+    <col min="45" max="45" width="30.64453125" style="14" customWidth="1"/>
     <col min="46" max="47" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:45" ht="14.7" hidden="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="AC1"/>
-      <c r="AD1" t="str">
-        <f>IFERROR(HLOOKUP(AD4,$AB$4:AC4,1,0),"OK")</f>
-        <v>OK</v>
-      </c>
-      <c r="AG1" t="str">
-        <f>IFERROR(HLOOKUP(AG4,$AB$4:AF4,1,0),"OK")</f>
-        <v>OK</v>
-      </c>
-      <c r="AJ1" t="str">
-        <f>IFERROR(HLOOKUP(AJ4,$AB$4:AI4,1,0),"OK")</f>
-        <v>OK</v>
-      </c>
-      <c r="AM1" t="str">
-        <f>IFERROR(HLOOKUP(AM4,$AB$4:AL4,1,0),"OK")</f>
-        <v>OK</v>
-      </c>
-      <c r="AP1" t="str">
-        <f>IFERROR(HLOOKUP(AP4,$AB$4:AO4,1,0),"OK")</f>
-        <v>OK</v>
-      </c>
-      <c r="AS1" t="str">
-        <f>IFERROR(HLOOKUP(AS4,$AB$4:AR4,1,0),"OK")</f>
-        <v>OK</v>
-      </c>
+      <c r="AD1"/>
+      <c r="AG1"/>
+      <c r="AJ1"/>
+      <c r="AM1"/>
+      <c r="AP1"/>
+      <c r="AS1"/>
     </row>
     <row r="2" spans="1:45" ht="14.7" hidden="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="AC2"/>
-      <c r="AD2">
-        <f>COUNTA(AD5:AD36)</f>
-        <v>0</v>
-      </c>
-      <c r="AG2">
-        <f>COUNTA(AG5:AG36)</f>
-        <v>0</v>
-      </c>
-      <c r="AJ2">
-        <f>COUNTA(AJ5:AJ36)</f>
-        <v>0</v>
-      </c>
-      <c r="AM2">
-        <f>COUNTA(AM5:AM36)</f>
-        <v>0</v>
-      </c>
-      <c r="AP2">
-        <f>COUNTA(AP5:AP36)</f>
-        <v>0</v>
-      </c>
-      <c r="AS2">
-        <f>COUNTA(AS5:AS36)</f>
-        <v>0</v>
-      </c>
+      <c r="AD2"/>
+      <c r="AG2"/>
+      <c r="AJ2"/>
+      <c r="AM2"/>
+      <c r="AP2"/>
+      <c r="AS2"/>
     </row>
     <row r="3" spans="1:45" ht="14.7" hidden="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="AC3"/>
-      <c r="AD3">
-        <f>COUNTA(AD39:AD79)</f>
-        <v>0</v>
-      </c>
-      <c r="AG3">
-        <f>COUNTA(AG39:AG79)</f>
-        <v>0</v>
-      </c>
-      <c r="AJ3">
-        <f>COUNTA(AJ39:AJ79)</f>
-        <v>0</v>
-      </c>
-      <c r="AM3">
-        <f>COUNTA(AM39:AM79)</f>
-        <v>0</v>
-      </c>
-      <c r="AP3">
-        <f>COUNTA(AP39:AP79)</f>
-        <v>0</v>
-      </c>
-      <c r="AS3">
-        <f>COUNTA(AS39:AS79)</f>
-        <v>0</v>
-      </c>
+      <c r="AD3"/>
+      <c r="AG3"/>
+      <c r="AJ3"/>
+      <c r="AM3"/>
+      <c r="AP3"/>
+      <c r="AS3"/>
     </row>
     <row r="4" spans="1:45" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="5">
@@ -7506,7 +6897,7 @@
     <row r="37" spans="1:45" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="16" t="str">
         <f>'Formulas OM'!A37</f>
-        <v>V - 7.7</v>
+        <v>V - 8.0</v>
       </c>
       <c r="AC37" s="2"/>
       <c r="AD37" s="2"/>
@@ -7651,7 +7042,7 @@
       <c r="AC49" s="1"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="BHw6+TLw4IvEnsl/DlmonKbCry9j3YpQcu/M+eaWDbjymaLD2D/8jJOxQCc6odAayKNEtuNA66HePN3+gr/ifA==" saltValue="hZUGRf9ePGHSfX6zGbHi8Q==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1" autoFilter="0"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="mGHJbEDqrvHZcdgX6Qajq7Q3PE6ZwqFjhWYfdKs/SKInvoil8mjXopB9WXs96Gam//4mRmUi3AxrugiicgbzUw==" saltValue="tiFaoNTJ4E+hnks3i0vW2Q==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1" autoFilter="0"/>
   <mergeCells count="2">
     <mergeCell ref="A5:A20"/>
     <mergeCell ref="A21:A36"/>
@@ -7663,115 +7054,61 @@
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <sheetPr codeName="Hoja8"/>
-  <dimension ref="A1:AS48"/>
+  <dimension ref="A1:AS47"/>
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="29" ySplit="4" topLeftCell="AD5" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="AG14" sqref="AG14"/>
-      <selection pane="topRight" activeCell="AG14" sqref="AG14"/>
-      <selection pane="bottomLeft" activeCell="AG14" sqref="AG14"/>
-      <selection pane="bottomRight" activeCell="AD5" sqref="AD5"/>
+      <selection activeCell="AD5" sqref="AD5"/>
+      <selection pane="topRight" activeCell="AD5" sqref="AD5"/>
+      <selection pane="bottomLeft" activeCell="AD5" sqref="AD5"/>
+      <selection pane="bottomRight" activeCell="AD4" sqref="AD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" zeroHeight="1" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="6.703125" customWidth="1"/>
+    <col min="1" max="1" width="6.64453125" customWidth="1"/>
     <col min="2" max="28" width="11.41015625" hidden="1" customWidth="1"/>
-    <col min="29" max="29" width="15.703125" style="1" customWidth="1"/>
-    <col min="30" max="30" width="30.703125" style="1" customWidth="1"/>
+    <col min="29" max="29" width="15.64453125" style="1" customWidth="1"/>
+    <col min="30" max="30" width="30.64453125" style="1" customWidth="1"/>
     <col min="31" max="32" width="0" hidden="1" customWidth="1"/>
-    <col min="33" max="33" width="30.703125" style="1" customWidth="1"/>
+    <col min="33" max="33" width="30.64453125" style="1" customWidth="1"/>
     <col min="34" max="35" width="0" hidden="1" customWidth="1"/>
-    <col min="36" max="36" width="30.703125" style="1" customWidth="1"/>
+    <col min="36" max="36" width="30.64453125" style="1" customWidth="1"/>
     <col min="37" max="38" width="0" hidden="1" customWidth="1"/>
-    <col min="39" max="39" width="30.703125" style="1" customWidth="1"/>
+    <col min="39" max="39" width="30.64453125" style="1" customWidth="1"/>
     <col min="40" max="41" width="0" hidden="1" customWidth="1"/>
-    <col min="42" max="42" width="30.703125" style="1" customWidth="1"/>
+    <col min="42" max="42" width="30.64453125" style="1" customWidth="1"/>
     <col min="43" max="44" width="0" hidden="1" customWidth="1"/>
-    <col min="45" max="45" width="30.703125" style="1" customWidth="1"/>
+    <col min="45" max="45" width="30.64453125" style="1" customWidth="1"/>
     <col min="46" max="47" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:45" ht="14.7" hidden="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="AC1"/>
-      <c r="AD1" t="str">
-        <f>IFERROR(HLOOKUP(AD4,$AB$4:AC4,1,0),"OK")</f>
-        <v>OK</v>
-      </c>
-      <c r="AG1" t="str">
-        <f>IFERROR(HLOOKUP(AG4,$AB$4:AF4,1,0),"OK")</f>
-        <v>OK</v>
-      </c>
-      <c r="AJ1" t="str">
-        <f>IFERROR(HLOOKUP(AJ4,$AB$4:AI4,1,0),"OK")</f>
-        <v>OK</v>
-      </c>
-      <c r="AM1" t="str">
-        <f>IFERROR(HLOOKUP(AM4,$AB$4:AL4,1,0),"OK")</f>
-        <v>OK</v>
-      </c>
-      <c r="AP1" t="str">
-        <f>IFERROR(HLOOKUP(AP4,$AB$4:AO4,1,0),"OK")</f>
-        <v>OK</v>
-      </c>
-      <c r="AS1" t="str">
-        <f>IFERROR(HLOOKUP(AS4,$AB$4:AR4,1,0),"OK")</f>
-        <v>OK</v>
-      </c>
+      <c r="AD1"/>
+      <c r="AG1"/>
+      <c r="AJ1"/>
+      <c r="AM1"/>
+      <c r="AP1"/>
+      <c r="AS1"/>
     </row>
     <row r="2" spans="1:45" ht="14.7" hidden="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="AC2"/>
-      <c r="AD2">
-        <f>COUNTA(AD5:AD36)</f>
-        <v>0</v>
-      </c>
-      <c r="AG2">
-        <f>COUNTA(AG5:AG36)</f>
-        <v>0</v>
-      </c>
-      <c r="AJ2">
-        <f>COUNTA(AJ5:AJ36)</f>
-        <v>0</v>
-      </c>
-      <c r="AM2">
-        <f>COUNTA(AM5:AM36)</f>
-        <v>0</v>
-      </c>
-      <c r="AP2">
-        <f>COUNTA(AP5:AP36)</f>
-        <v>0</v>
-      </c>
-      <c r="AS2">
-        <f>COUNTA(AS5:AS36)</f>
-        <v>0</v>
-      </c>
+      <c r="AD2"/>
+      <c r="AG2"/>
+      <c r="AJ2"/>
+      <c r="AM2"/>
+      <c r="AP2"/>
+      <c r="AS2"/>
     </row>
     <row r="3" spans="1:45" ht="14.7" hidden="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="AC3"/>
-      <c r="AD3">
-        <f>COUNTA(AD39:AD79)</f>
-        <v>0</v>
-      </c>
-      <c r="AG3">
-        <f>COUNTA(AG39:AG79)</f>
-        <v>0</v>
-      </c>
-      <c r="AJ3">
-        <f>COUNTA(AJ39:AJ79)</f>
-        <v>0</v>
-      </c>
-      <c r="AM3">
-        <f>COUNTA(AM39:AM79)</f>
-        <v>0</v>
-      </c>
-      <c r="AP3">
-        <f>COUNTA(AP39:AP79)</f>
-        <v>0</v>
-      </c>
-      <c r="AS3">
-        <f>COUNTA(AS39:AS79)</f>
-        <v>0</v>
-      </c>
+      <c r="AD3"/>
+      <c r="AG3"/>
+      <c r="AJ3"/>
+      <c r="AM3"/>
+      <c r="AP3"/>
+      <c r="AS3"/>
     </row>
     <row r="4" spans="1:45" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="5">
@@ -8179,7 +7516,7 @@
     <row r="37" spans="1:45" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="16" t="str">
         <f>'Formulas OM'!A37</f>
-        <v>V - 7.7</v>
+        <v>V - 8.0</v>
       </c>
       <c r="AC37" s="2"/>
       <c r="AD37" s="2"/>
@@ -8222,7 +7559,7 @@
       <c r="AP40" s="10"/>
       <c r="AS40" s="10"/>
     </row>
-    <row r="41" spans="1:45" x14ac:dyDescent="0.5">
+    <row r="41" spans="1:45" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="AC41" s="9" t="s">
         <v>34</v>
       </c>
@@ -8233,27 +7570,27 @@
       <c r="AP41" s="10"/>
       <c r="AS41" s="10"/>
     </row>
-    <row r="42" spans="1:45" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="AC42" s="9" t="s">
-        <v>166</v>
-      </c>
-      <c r="AD42" s="10"/>
-      <c r="AG42" s="10"/>
-      <c r="AJ42" s="10"/>
-      <c r="AM42" s="10"/>
-      <c r="AP42" s="10"/>
-      <c r="AS42" s="10"/>
+    <row r="42" spans="1:45" x14ac:dyDescent="0.5">
+      <c r="AC42" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="AD42" s="21"/>
+      <c r="AG42" s="21"/>
+      <c r="AJ42" s="21"/>
+      <c r="AM42" s="21"/>
+      <c r="AP42" s="21"/>
+      <c r="AS42" s="21"/>
     </row>
     <row r="43" spans="1:45" x14ac:dyDescent="0.5">
-      <c r="AC43" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="AD43" s="21"/>
-      <c r="AG43" s="21"/>
-      <c r="AJ43" s="21"/>
-      <c r="AM43" s="21"/>
-      <c r="AP43" s="21"/>
-      <c r="AS43" s="21"/>
+      <c r="AC43" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD43" s="10"/>
+      <c r="AG43" s="10"/>
+      <c r="AJ43" s="10"/>
+      <c r="AM43" s="10"/>
+      <c r="AP43" s="10"/>
+      <c r="AS43" s="10"/>
     </row>
     <row r="44" spans="1:45" x14ac:dyDescent="0.5">
       <c r="AC44" s="9" t="s">
@@ -8268,7 +7605,7 @@
     </row>
     <row r="45" spans="1:45" x14ac:dyDescent="0.5">
       <c r="AC45" s="9" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="AD45" s="10"/>
       <c r="AG45" s="10"/>
@@ -8277,31 +7614,20 @@
       <c r="AP45" s="10"/>
       <c r="AS45" s="10"/>
     </row>
-    <row r="46" spans="1:45" x14ac:dyDescent="0.5">
-      <c r="AC46" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="AD46" s="10"/>
-      <c r="AG46" s="10"/>
-      <c r="AJ46" s="10"/>
-      <c r="AM46" s="10"/>
-      <c r="AP46" s="10"/>
-      <c r="AS46" s="10"/>
-    </row>
-    <row r="47" spans="1:45" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="AC47" s="11" t="s">
+    <row r="46" spans="1:45" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC46" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="AD47" s="12"/>
-      <c r="AG47" s="12"/>
-      <c r="AJ47" s="12"/>
-      <c r="AM47" s="12"/>
-      <c r="AP47" s="12"/>
-      <c r="AS47" s="12"/>
-    </row>
-    <row r="48" spans="1:45" x14ac:dyDescent="0.5"/>
+      <c r="AD46" s="12"/>
+      <c r="AG46" s="12"/>
+      <c r="AJ46" s="12"/>
+      <c r="AM46" s="12"/>
+      <c r="AP46" s="12"/>
+      <c r="AS46" s="12"/>
+    </row>
+    <row r="47" spans="1:45" x14ac:dyDescent="0.5"/>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="UNNs13oxSNFvKyDYTc/+spqIOAS6TIjoCsCvcwYKFP4ptgzsuEUz8QI3kYow7Hfanwj2Rn3qxn+V8WfD6usIPQ==" saltValue="ivlCcEHhFK/Z/H6KxPcrfw==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1" autoFilter="0"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="6YlU1uZ98Mtx2qqrzEd6gxDm96w0IbLAIQ22JJZbuQfwBy+Gs6/FoGfO+GEG09PVlDeah46Si2dc3avBljOhGg==" saltValue="3lzqRZJ6Z3J8SLBCc/YB8w==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1" autoFilter="0"/>
   <mergeCells count="2">
     <mergeCell ref="A5:A20"/>
     <mergeCell ref="A21:A36"/>

</xml_diff>